<commit_message>
Corrected version of full corpus data, and corresponding stats and descriptions.
</commit_message>
<xml_diff>
--- a/full/stats/TypeMentionStats.xlsx
+++ b/full/stats/TypeMentionStats.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunilmohan/Home/Projects/MedMentions/full/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02381186-825C-E34A-96E4-D559EC76BDAE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12160B0D-12D7-444A-A29D-89D8008E303E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20780" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{900A78CF-1263-6D42-B34D-1DC694662144}"/>
+    <workbookView xWindow="40080" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{900A78CF-1263-6D42-B34D-1DC694662144}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="279">
   <si>
     <t>Nbr Semantic Types</t>
   </si>
   <si>
-    <t>(incl. UnknownType)</t>
-  </si>
-  <si>
     <t>Nbr Annotated Docs</t>
   </si>
   <si>
@@ -861,10 +858,10 @@
     <t>Mapped Concepts</t>
   </si>
   <si>
-    <t>Nbr Concepts in UMLS 2017-AA Active</t>
-  </si>
-  <si>
     <t>UMLS 2017-AA Active</t>
+  </si>
+  <si>
+    <t>Nbr Concepts in UMLS</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1550,7 @@
   <dimension ref="A1:N138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1581,9 +1578,6 @@
       <c r="C1" s="2">
         <v>128</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1594,53 +1588,50 @@
       </c>
       <c r="D2" s="3"/>
       <c r="G2" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H2" s="38"/>
       <c r="I2" s="38"/>
       <c r="J2" s="34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
         <v>4392</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H3" s="40"/>
       <c r="I3" s="41"/>
       <c r="J3" s="34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>34720</v>
-      </c>
-      <c r="D4" s="4">
-        <f>C4/C2</f>
-        <v>1.0614088612966062E-2</v>
-      </c>
+        <v>34728</v>
+      </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>351813</v>
+        <v>352594</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1674,17 +1665,17 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F9" s="43"/>
       <c r="G9" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L9" s="36"/>
       <c r="M9" s="36"/>
@@ -1692,46 +1683,46 @@
     </row>
     <row r="10" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="H10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="J10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="M10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1739,10 +1730,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>19</v>
       </c>
       <c r="D11" s="17">
         <v>1</v>
@@ -1775,7 +1766,7 @@
         <v>4380</v>
       </c>
       <c r="N11" s="19">
-        <v>99473</v>
+        <v>99600</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1783,10 +1774,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>21</v>
       </c>
       <c r="D12" s="23">
         <v>2</v>
@@ -1807,7 +1798,7 @@
         <v>2615</v>
       </c>
       <c r="J12" s="25">
-        <v>7253</v>
+        <v>7254</v>
       </c>
       <c r="K12" s="25">
         <v>5128</v>
@@ -1819,7 +1810,7 @@
         <v>4283</v>
       </c>
       <c r="N12" s="25">
-        <v>48502</v>
+        <v>48531</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1827,10 +1818,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>23</v>
       </c>
       <c r="D13" s="23">
         <v>3</v>
@@ -1871,10 +1862,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>24</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>25</v>
       </c>
       <c r="D14" s="23">
         <v>4</v>
@@ -1915,10 +1906,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>27</v>
       </c>
       <c r="D15" s="23">
         <v>4</v>
@@ -1959,10 +1950,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="D16" s="23">
         <v>3</v>
@@ -2003,10 +1994,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="D17" s="23">
         <v>3</v>
@@ -2039,7 +2030,7 @@
         <v>4142</v>
       </c>
       <c r="N17" s="25">
-        <v>37667</v>
+        <v>37694</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -2047,10 +2038,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>33</v>
       </c>
       <c r="D18" s="23">
         <v>4</v>
@@ -2071,7 +2062,7 @@
         <v>1840</v>
       </c>
       <c r="J18" s="25">
-        <v>5672</v>
+        <v>5683</v>
       </c>
       <c r="K18" s="25">
         <v>3760</v>
@@ -2083,7 +2074,7 @@
         <v>3593</v>
       </c>
       <c r="N18" s="25">
-        <v>26283</v>
+        <v>26310</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -2091,10 +2082,10 @@
         <v>9</v>
       </c>
       <c r="B19" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>35</v>
       </c>
       <c r="D19" s="23">
         <v>5</v>
@@ -2115,7 +2106,7 @@
         <v>1546</v>
       </c>
       <c r="J19" s="25">
-        <v>5105</v>
+        <v>5111</v>
       </c>
       <c r="K19" s="25">
         <v>908</v>
@@ -2127,7 +2118,7 @@
         <v>1546</v>
       </c>
       <c r="N19" s="25">
-        <v>5105</v>
+        <v>5111</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -2135,10 +2126,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>37</v>
       </c>
       <c r="D20" s="23">
         <v>5</v>
@@ -2179,10 +2170,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>38</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>39</v>
       </c>
       <c r="D21" s="23">
         <v>5</v>
@@ -2203,7 +2194,7 @@
         <v>2145</v>
       </c>
       <c r="J21" s="25">
-        <v>11423</v>
+        <v>11433</v>
       </c>
       <c r="K21" s="25">
         <v>1618</v>
@@ -2215,7 +2206,7 @@
         <v>2145</v>
       </c>
       <c r="N21" s="25">
-        <v>11423</v>
+        <v>11433</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -2223,10 +2214,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="D22" s="23">
         <v>4</v>
@@ -2267,10 +2258,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="D23" s="23">
         <v>5</v>
@@ -2311,10 +2302,10 @@
         <v>14</v>
       </c>
       <c r="B24" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>45</v>
       </c>
       <c r="D24" s="23">
         <v>4</v>
@@ -2355,10 +2346,10 @@
         <v>15</v>
       </c>
       <c r="B25" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>47</v>
       </c>
       <c r="D25" s="23">
         <v>4</v>
@@ -2399,10 +2390,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>49</v>
       </c>
       <c r="D26" s="23">
         <v>3</v>
@@ -2423,7 +2414,7 @@
         <v>125</v>
       </c>
       <c r="J26" s="25">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K26" s="25">
         <v>37</v>
@@ -2435,7 +2426,7 @@
         <v>125</v>
       </c>
       <c r="N26" s="25">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -2443,10 +2434,10 @@
         <v>17</v>
       </c>
       <c r="B27" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>50</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>51</v>
       </c>
       <c r="D27" s="23">
         <v>2</v>
@@ -2467,7 +2458,7 @@
         <v>900</v>
       </c>
       <c r="J27" s="25">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="K27" s="25">
         <v>6395</v>
@@ -2479,7 +2470,7 @@
         <v>4206</v>
       </c>
       <c r="N27" s="25">
-        <v>50679</v>
+        <v>50777</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -2487,10 +2478,10 @@
         <v>18</v>
       </c>
       <c r="B28" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>52</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>53</v>
       </c>
       <c r="D28" s="23">
         <v>3</v>
@@ -2511,7 +2502,7 @@
         <v>521</v>
       </c>
       <c r="J28" s="25">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="K28" s="25">
         <v>274</v>
@@ -2523,7 +2514,7 @@
         <v>521</v>
       </c>
       <c r="N28" s="25">
-        <v>1895</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -2531,10 +2522,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>54</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>55</v>
       </c>
       <c r="D29" s="23">
         <v>3</v>
@@ -2575,10 +2566,10 @@
         <v>20</v>
       </c>
       <c r="B30" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="22" t="s">
         <v>56</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>57</v>
       </c>
       <c r="D30" s="23">
         <v>4</v>
@@ -2619,10 +2610,10 @@
         <v>21</v>
       </c>
       <c r="B31" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="D31" s="23">
         <v>3</v>
@@ -2643,7 +2634,7 @@
         <v>956</v>
       </c>
       <c r="J31" s="25">
-        <v>2831</v>
+        <v>2834</v>
       </c>
       <c r="K31" s="25">
         <v>5893</v>
@@ -2655,7 +2646,7 @@
         <v>4115</v>
       </c>
       <c r="N31" s="25">
-        <v>46269</v>
+        <v>46365</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -2663,10 +2654,10 @@
         <v>22</v>
       </c>
       <c r="B32" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>60</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>61</v>
       </c>
       <c r="D32" s="23">
         <v>4</v>
@@ -2699,7 +2690,7 @@
         <v>3955</v>
       </c>
       <c r="N32" s="25">
-        <v>43438</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -2707,10 +2698,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>63</v>
       </c>
       <c r="D33" s="23">
         <v>5</v>
@@ -2731,7 +2722,7 @@
         <v>581</v>
       </c>
       <c r="J33" s="25">
-        <v>1307</v>
+        <v>1312</v>
       </c>
       <c r="K33" s="25">
         <v>2419</v>
@@ -2743,7 +2734,7 @@
         <v>2984</v>
       </c>
       <c r="N33" s="25">
-        <v>18949</v>
+        <v>18962</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -2751,10 +2742,10 @@
         <v>24</v>
       </c>
       <c r="B34" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>64</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="D34" s="23">
         <v>6</v>
@@ -2775,7 +2766,7 @@
         <v>1032</v>
       </c>
       <c r="J34" s="25">
-        <v>2713</v>
+        <v>2715</v>
       </c>
       <c r="K34" s="25">
         <v>650</v>
@@ -2787,7 +2778,7 @@
         <v>1645</v>
       </c>
       <c r="N34" s="25">
-        <v>5946</v>
+        <v>5950</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -2795,10 +2786,10 @@
         <v>25</v>
       </c>
       <c r="B35" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="D35" s="23">
         <v>7</v>
@@ -2819,7 +2810,7 @@
         <v>838</v>
       </c>
       <c r="J35" s="25">
-        <v>3233</v>
+        <v>3235</v>
       </c>
       <c r="K35" s="25">
         <v>337</v>
@@ -2831,7 +2822,7 @@
         <v>838</v>
       </c>
       <c r="N35" s="25">
-        <v>3233</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -2839,10 +2830,10 @@
         <v>26</v>
       </c>
       <c r="B36" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="D36" s="23">
         <v>6</v>
@@ -2883,10 +2874,10 @@
         <v>27</v>
       </c>
       <c r="B37" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="22" t="s">
         <v>70</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>71</v>
       </c>
       <c r="D37" s="23">
         <v>6</v>
@@ -2907,7 +2898,7 @@
         <v>809</v>
       </c>
       <c r="J37" s="25">
-        <v>3089</v>
+        <v>3090</v>
       </c>
       <c r="K37" s="25">
         <v>491</v>
@@ -2919,7 +2910,7 @@
         <v>809</v>
       </c>
       <c r="N37" s="25">
-        <v>3089</v>
+        <v>3090</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -2927,10 +2918,10 @@
         <v>28</v>
       </c>
       <c r="B38" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>73</v>
       </c>
       <c r="D38" s="23">
         <v>6</v>
@@ -2951,7 +2942,7 @@
         <v>1025</v>
       </c>
       <c r="J38" s="25">
-        <v>3470</v>
+        <v>3471</v>
       </c>
       <c r="K38" s="25">
         <v>782</v>
@@ -2963,7 +2954,7 @@
         <v>1420</v>
       </c>
       <c r="N38" s="25">
-        <v>6908</v>
+        <v>6911</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -2971,10 +2962,10 @@
         <v>29</v>
       </c>
       <c r="B39" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>74</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>75</v>
       </c>
       <c r="D39" s="23">
         <v>7</v>
@@ -2995,7 +2986,7 @@
         <v>931</v>
       </c>
       <c r="J39" s="25">
-        <v>3438</v>
+        <v>3440</v>
       </c>
       <c r="K39" s="25">
         <v>204</v>
@@ -3007,7 +2998,7 @@
         <v>931</v>
       </c>
       <c r="N39" s="25">
-        <v>3438</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -3015,10 +3006,10 @@
         <v>30</v>
       </c>
       <c r="B40" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="D40" s="23">
         <v>5</v>
@@ -3039,7 +3030,7 @@
         <v>1311</v>
       </c>
       <c r="J40" s="25">
-        <v>3962</v>
+        <v>3964</v>
       </c>
       <c r="K40" s="25">
         <v>3090</v>
@@ -3051,7 +3042,7 @@
         <v>2941</v>
       </c>
       <c r="N40" s="25">
-        <v>23543</v>
+        <v>23623</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -3059,10 +3050,10 @@
         <v>31</v>
       </c>
       <c r="B41" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="22" t="s">
         <v>78</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>79</v>
       </c>
       <c r="D41" s="23">
         <v>6</v>
@@ -3083,7 +3074,7 @@
         <v>1925</v>
       </c>
       <c r="J41" s="25">
-        <v>11693</v>
+        <v>11754</v>
       </c>
       <c r="K41" s="25">
         <v>2524</v>
@@ -3095,7 +3086,7 @@
         <v>2574</v>
       </c>
       <c r="N41" s="25">
-        <v>18700</v>
+        <v>18777</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -3103,10 +3094,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>80</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>81</v>
       </c>
       <c r="D42" s="23">
         <v>7</v>
@@ -3127,7 +3118,7 @@
         <v>400</v>
       </c>
       <c r="J42" s="25">
-        <v>2272</v>
+        <v>2284</v>
       </c>
       <c r="K42" s="25">
         <v>243</v>
@@ -3139,7 +3130,7 @@
         <v>400</v>
       </c>
       <c r="N42" s="25">
-        <v>2272</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
@@ -3147,10 +3138,10 @@
         <v>33</v>
       </c>
       <c r="B43" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="D43" s="23">
         <v>7</v>
@@ -3171,7 +3162,7 @@
         <v>705</v>
       </c>
       <c r="J43" s="25">
-        <v>4735</v>
+        <v>4739</v>
       </c>
       <c r="K43" s="25">
         <v>604</v>
@@ -3183,7 +3174,7 @@
         <v>705</v>
       </c>
       <c r="N43" s="25">
-        <v>4735</v>
+        <v>4739</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -3191,10 +3182,10 @@
         <v>34</v>
       </c>
       <c r="B44" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="D44" s="23">
         <v>6</v>
@@ -3212,10 +3203,10 @@
         <v>4.7662694775435298E-2</v>
       </c>
       <c r="I44" s="25">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="J44" s="25">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="K44" s="25">
         <v>104</v>
@@ -3224,10 +3215,10 @@
         <v>4.7662694775435298E-2</v>
       </c>
       <c r="M44" s="25">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N44" s="25">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -3235,10 +3226,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="22" t="s">
         <v>86</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>87</v>
       </c>
       <c r="D45" s="23">
         <v>6</v>
@@ -3279,10 +3270,10 @@
         <v>36</v>
       </c>
       <c r="B46" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>88</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>89</v>
       </c>
       <c r="D46" s="23">
         <v>1</v>
@@ -3306,16 +3297,16 @@
         <v>109</v>
       </c>
       <c r="K46" s="25">
-        <v>22543</v>
+        <v>22551</v>
       </c>
       <c r="L46" s="26">
-        <v>8.9047648767600698E-3</v>
+        <v>8.9079249760819906E-3</v>
       </c>
       <c r="M46" s="25">
         <v>4392</v>
       </c>
       <c r="N46" s="25">
-        <v>250210</v>
+        <v>250857</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -3323,10 +3314,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="22" t="s">
         <v>90</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>91</v>
       </c>
       <c r="D47" s="23">
         <v>2</v>
@@ -3350,16 +3341,16 @@
         <v>79</v>
       </c>
       <c r="K47" s="25">
-        <v>11722</v>
+        <v>11727</v>
       </c>
       <c r="L47" s="26">
-        <v>5.7885562189202103E-3</v>
+        <v>5.79102531814343E-3</v>
       </c>
       <c r="M47" s="25">
         <v>4013</v>
       </c>
       <c r="N47" s="25">
-        <v>82642</v>
+        <v>82788</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -3367,10 +3358,10 @@
         <v>38</v>
       </c>
       <c r="B48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="22" t="s">
         <v>92</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>93</v>
       </c>
       <c r="D48" s="23">
         <v>3</v>
@@ -3403,7 +3394,7 @@
         <v>1727</v>
       </c>
       <c r="N48" s="25">
-        <v>12853</v>
+        <v>12855</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3411,10 +3402,10 @@
         <v>39</v>
       </c>
       <c r="B49" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="22" t="s">
         <v>94</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>95</v>
       </c>
       <c r="D49" s="23">
         <v>4</v>
@@ -3455,10 +3446,10 @@
         <v>40</v>
       </c>
       <c r="B50" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="22" t="s">
         <v>96</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>97</v>
       </c>
       <c r="D50" s="23">
         <v>4</v>
@@ -3499,10 +3490,10 @@
         <v>41</v>
       </c>
       <c r="B51" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="22" t="s">
         <v>98</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>99</v>
       </c>
       <c r="D51" s="23">
         <v>4</v>
@@ -3543,10 +3534,10 @@
         <v>42</v>
       </c>
       <c r="B52" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="22" t="s">
         <v>100</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>101</v>
       </c>
       <c r="D52" s="23">
         <v>4</v>
@@ -3567,7 +3558,7 @@
         <v>247</v>
       </c>
       <c r="J52" s="25">
-        <v>1798</v>
+        <v>1799</v>
       </c>
       <c r="K52" s="25">
         <v>1243</v>
@@ -3579,7 +3570,7 @@
         <v>1428</v>
       </c>
       <c r="N52" s="25">
-        <v>8640</v>
+        <v>8642</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
@@ -3587,10 +3578,10 @@
         <v>43</v>
       </c>
       <c r="B53" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="22" t="s">
         <v>102</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>103</v>
       </c>
       <c r="D53" s="23">
         <v>5</v>
@@ -3631,10 +3622,10 @@
         <v>44</v>
       </c>
       <c r="B54" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="D54" s="23">
         <v>5</v>
@@ -3675,10 +3666,10 @@
         <v>45</v>
       </c>
       <c r="B55" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="22" t="s">
         <v>106</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>107</v>
       </c>
       <c r="D55" s="23">
         <v>5</v>
@@ -3711,7 +3702,7 @@
         <v>1083</v>
       </c>
       <c r="N55" s="25">
-        <v>4306</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -3719,10 +3710,10 @@
         <v>46</v>
       </c>
       <c r="B56" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>109</v>
       </c>
       <c r="D56" s="23">
         <v>6</v>
@@ -3755,7 +3746,7 @@
         <v>1037</v>
       </c>
       <c r="N56" s="25">
-        <v>3877</v>
+        <v>3878</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3763,10 +3754,10 @@
         <v>47</v>
       </c>
       <c r="B57" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="22" t="s">
         <v>110</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>111</v>
       </c>
       <c r="D57" s="23">
         <v>7</v>
@@ -3807,10 +3798,10 @@
         <v>48</v>
       </c>
       <c r="B58" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="22" t="s">
         <v>112</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>113</v>
       </c>
       <c r="D58" s="23">
         <v>7</v>
@@ -3851,10 +3842,10 @@
         <v>49</v>
       </c>
       <c r="B59" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="22" t="s">
         <v>114</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>115</v>
       </c>
       <c r="D59" s="23">
         <v>7</v>
@@ -3895,10 +3886,10 @@
         <v>50</v>
       </c>
       <c r="B60" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="22" t="s">
         <v>116</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="D60" s="23">
         <v>7</v>
@@ -3939,10 +3930,10 @@
         <v>51</v>
       </c>
       <c r="B61" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="22" t="s">
         <v>118</v>
-      </c>
-      <c r="C61" s="22" t="s">
-        <v>119</v>
       </c>
       <c r="D61" s="23">
         <v>7</v>
@@ -3963,7 +3954,7 @@
         <v>635</v>
       </c>
       <c r="J61" s="25">
-        <v>2299</v>
+        <v>2300</v>
       </c>
       <c r="K61" s="25">
         <v>161</v>
@@ -3975,7 +3966,7 @@
         <v>946</v>
       </c>
       <c r="N61" s="25">
-        <v>3031</v>
+        <v>3032</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -3983,10 +3974,10 @@
         <v>52</v>
       </c>
       <c r="B62" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>121</v>
       </c>
       <c r="D62" s="23">
         <v>8</v>
@@ -4027,10 +4018,10 @@
         <v>53</v>
       </c>
       <c r="B63" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="22" t="s">
         <v>122</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>123</v>
       </c>
       <c r="D63" s="23">
         <v>3</v>
@@ -4063,7 +4054,7 @@
         <v>2538</v>
       </c>
       <c r="N63" s="25">
-        <v>20762</v>
+        <v>20791</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -4071,10 +4062,10 @@
         <v>54</v>
       </c>
       <c r="B64" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="22" t="s">
         <v>124</v>
-      </c>
-      <c r="C64" s="22" t="s">
-        <v>125</v>
       </c>
       <c r="D64" s="23">
         <v>4</v>
@@ -4115,10 +4106,10 @@
         <v>55</v>
       </c>
       <c r="B65" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" s="22" t="s">
         <v>126</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>127</v>
       </c>
       <c r="D65" s="23">
         <v>4</v>
@@ -4151,7 +4142,7 @@
         <v>2461</v>
       </c>
       <c r="N65" s="25">
-        <v>19551</v>
+        <v>19580</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -4159,10 +4150,10 @@
         <v>56</v>
       </c>
       <c r="B66" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="C66" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="D66" s="23">
         <v>5</v>
@@ -4183,7 +4174,7 @@
         <v>1364</v>
       </c>
       <c r="J66" s="25">
-        <v>6299</v>
+        <v>6314</v>
       </c>
       <c r="K66" s="25">
         <v>1029</v>
@@ -4195,7 +4186,7 @@
         <v>1364</v>
       </c>
       <c r="N66" s="25">
-        <v>6299</v>
+        <v>6314</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -4203,10 +4194,10 @@
         <v>57</v>
       </c>
       <c r="B67" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="C67" s="22" t="s">
-        <v>131</v>
       </c>
       <c r="D67" s="23">
         <v>5</v>
@@ -4227,7 +4218,7 @@
         <v>614</v>
       </c>
       <c r="J67" s="25">
-        <v>1581</v>
+        <v>1584</v>
       </c>
       <c r="K67" s="25">
         <v>174</v>
@@ -4239,7 +4230,7 @@
         <v>614</v>
       </c>
       <c r="N67" s="25">
-        <v>1581</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -4247,10 +4238,10 @@
         <v>58</v>
       </c>
       <c r="B68" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="22" t="s">
         <v>132</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>133</v>
       </c>
       <c r="D68" s="23">
         <v>5</v>
@@ -4271,7 +4262,7 @@
         <v>1031</v>
       </c>
       <c r="J68" s="25">
-        <v>5536</v>
+        <v>5543</v>
       </c>
       <c r="K68" s="25">
         <v>327</v>
@@ -4283,7 +4274,7 @@
         <v>1031</v>
       </c>
       <c r="N68" s="25">
-        <v>5536</v>
+        <v>5543</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4291,10 +4282,10 @@
         <v>59</v>
       </c>
       <c r="B69" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="22" t="s">
         <v>134</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>135</v>
       </c>
       <c r="D69" s="23">
         <v>5</v>
@@ -4315,7 +4306,7 @@
         <v>456</v>
       </c>
       <c r="J69" s="25">
-        <v>1590</v>
+        <v>1594</v>
       </c>
       <c r="K69" s="25">
         <v>317</v>
@@ -4327,7 +4318,7 @@
         <v>456</v>
       </c>
       <c r="N69" s="25">
-        <v>1590</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -4335,10 +4326,10 @@
         <v>60</v>
       </c>
       <c r="B70" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="22" t="s">
         <v>136</v>
-      </c>
-      <c r="C70" s="22" t="s">
-        <v>137</v>
       </c>
       <c r="D70" s="23">
         <v>5</v>
@@ -4379,10 +4370,10 @@
         <v>61</v>
       </c>
       <c r="B71" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="C71" s="22" t="s">
-        <v>139</v>
       </c>
       <c r="D71" s="23">
         <v>4</v>
@@ -4423,10 +4414,10 @@
         <v>62</v>
       </c>
       <c r="B72" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" s="22" t="s">
         <v>140</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>141</v>
       </c>
       <c r="D72" s="23">
         <v>5</v>
@@ -4467,10 +4458,10 @@
         <v>63</v>
       </c>
       <c r="B73" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="D73" s="23">
         <v>5</v>
@@ -4511,10 +4502,10 @@
         <v>64</v>
       </c>
       <c r="B74" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="22" t="s">
         <v>144</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>145</v>
       </c>
       <c r="D74" s="23">
         <v>3</v>
@@ -4535,7 +4526,7 @@
         <v>1156</v>
       </c>
       <c r="J74" s="25">
-        <v>3606</v>
+        <v>3615</v>
       </c>
       <c r="K74" s="25">
         <v>969</v>
@@ -4547,7 +4538,7 @@
         <v>1620</v>
       </c>
       <c r="N74" s="25">
-        <v>6438</v>
+        <v>6448</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -4555,10 +4546,10 @@
         <v>65</v>
       </c>
       <c r="B75" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" s="22" t="s">
         <v>146</v>
-      </c>
-      <c r="C75" s="22" t="s">
-        <v>147</v>
       </c>
       <c r="D75" s="23">
         <v>4</v>
@@ -4579,7 +4570,7 @@
         <v>565</v>
       </c>
       <c r="J75" s="25">
-        <v>2386</v>
+        <v>2387</v>
       </c>
       <c r="K75" s="25">
         <v>468</v>
@@ -4591,7 +4582,7 @@
         <v>565</v>
       </c>
       <c r="N75" s="25">
-        <v>2406</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -4599,10 +4590,10 @@
         <v>66</v>
       </c>
       <c r="B76" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" s="22" t="s">
         <v>148</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>149</v>
       </c>
       <c r="D76" s="23">
         <v>5</v>
@@ -4643,10 +4634,10 @@
         <v>67</v>
       </c>
       <c r="B77" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77" s="22" t="s">
         <v>150</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>151</v>
       </c>
       <c r="D77" s="23">
         <v>4</v>
@@ -4687,10 +4678,10 @@
         <v>68</v>
       </c>
       <c r="B78" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="22" t="s">
         <v>152</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>153</v>
       </c>
       <c r="D78" s="23">
         <v>4</v>
@@ -4731,10 +4722,10 @@
         <v>69</v>
       </c>
       <c r="B79" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="22" t="s">
         <v>154</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>155</v>
       </c>
       <c r="D79" s="23">
         <v>3</v>
@@ -4755,19 +4746,19 @@
         <v>676</v>
       </c>
       <c r="J79" s="25">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="K79" s="25">
-        <v>5977</v>
+        <v>5982</v>
       </c>
       <c r="L79" s="26">
-        <v>1.31808759317249E-2</v>
+        <v>1.3191902262603E-2</v>
       </c>
       <c r="M79" s="25">
         <v>2928</v>
       </c>
       <c r="N79" s="25">
-        <v>42528</v>
+        <v>42633</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4775,10 +4766,10 @@
         <v>70</v>
       </c>
       <c r="B80" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="22" t="s">
         <v>156</v>
-      </c>
-      <c r="C80" s="22" t="s">
-        <v>157</v>
       </c>
       <c r="D80" s="23">
         <v>4</v>
@@ -4819,10 +4810,10 @@
         <v>71</v>
       </c>
       <c r="B81" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="22" t="s">
         <v>158</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>159</v>
       </c>
       <c r="D81" s="23">
         <v>4</v>
@@ -4846,16 +4837,16 @@
         <v>289</v>
       </c>
       <c r="K81" s="25">
-        <v>5611</v>
+        <v>5616</v>
       </c>
       <c r="L81" s="26">
-        <v>1.2887089254174901E-2</v>
+        <v>1.2898573026456301E-2</v>
       </c>
       <c r="M81" s="25">
         <v>2734</v>
       </c>
       <c r="N81" s="25">
-        <v>38133</v>
+        <v>38237</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -4863,10 +4854,10 @@
         <v>72</v>
       </c>
       <c r="B82" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" s="22" t="s">
         <v>160</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>161</v>
       </c>
       <c r="D82" s="23">
         <v>5</v>
@@ -4887,19 +4878,19 @@
         <v>275</v>
       </c>
       <c r="J82" s="25">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="K82" s="25">
-        <v>4908</v>
+        <v>4913</v>
       </c>
       <c r="L82" s="26">
-        <v>1.26550945264395E-2</v>
+        <v>1.26679868395268E-2</v>
       </c>
       <c r="M82" s="25">
         <v>2506</v>
       </c>
       <c r="N82" s="25">
-        <v>31481</v>
+        <v>31583</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -4907,10 +4898,10 @@
         <v>73</v>
       </c>
       <c r="B83" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" s="22" t="s">
         <v>162</v>
-      </c>
-      <c r="C83" s="22" t="s">
-        <v>163</v>
       </c>
       <c r="D83" s="23">
         <v>6</v>
@@ -4931,19 +4922,19 @@
         <v>1436</v>
       </c>
       <c r="J83" s="25">
-        <v>10277</v>
+        <v>10282</v>
       </c>
       <c r="K83" s="25">
-        <v>4537</v>
+        <v>4541</v>
       </c>
       <c r="L83" s="26">
-        <v>1.19573782848528E-2</v>
+        <v>1.1967920386051699E-2</v>
       </c>
       <c r="M83" s="25">
         <v>2370</v>
       </c>
       <c r="N83" s="25">
-        <v>27781</v>
+        <v>27829</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -4951,10 +4942,10 @@
         <v>74</v>
       </c>
       <c r="B84" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C84" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="C84" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="D84" s="23">
         <v>7</v>
@@ -4966,28 +4957,28 @@
         <v>12410</v>
       </c>
       <c r="G84" s="25">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="H84" s="26">
-        <v>2.1514907332796099E-2</v>
+        <v>2.16760676873489E-2</v>
       </c>
       <c r="I84" s="25">
         <v>548</v>
       </c>
       <c r="J84" s="25">
-        <v>2536</v>
+        <v>2570</v>
       </c>
       <c r="K84" s="25">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="L84" s="26">
-        <v>2.1514907332796099E-2</v>
+        <v>2.16760676873489E-2</v>
       </c>
       <c r="M84" s="25">
         <v>548</v>
       </c>
       <c r="N84" s="25">
-        <v>2536</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -4995,10 +4986,10 @@
         <v>75</v>
       </c>
       <c r="B85" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C85" s="22" t="s">
         <v>166</v>
-      </c>
-      <c r="C85" s="22" t="s">
-        <v>167</v>
       </c>
       <c r="D85" s="23">
         <v>7</v>
@@ -5010,28 +5001,28 @@
         <v>142043</v>
       </c>
       <c r="G85" s="25">
-        <v>2471</v>
+        <v>2473</v>
       </c>
       <c r="H85" s="26">
-        <v>1.7396140605309598E-2</v>
+        <v>1.7410220848616199E-2</v>
       </c>
       <c r="I85" s="25">
         <v>1620</v>
       </c>
       <c r="J85" s="25">
-        <v>14976</v>
+        <v>14985</v>
       </c>
       <c r="K85" s="25">
-        <v>2471</v>
+        <v>2473</v>
       </c>
       <c r="L85" s="26">
-        <v>1.7396140605309598E-2</v>
+        <v>1.7410220848616199E-2</v>
       </c>
       <c r="M85" s="25">
         <v>1620</v>
       </c>
       <c r="N85" s="25">
-        <v>14976</v>
+        <v>14985</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -5039,10 +5030,10 @@
         <v>76</v>
       </c>
       <c r="B86" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="22" t="s">
         <v>168</v>
-      </c>
-      <c r="C86" s="22" t="s">
-        <v>169</v>
       </c>
       <c r="D86" s="23">
         <v>6</v>
@@ -5054,28 +5045,28 @@
         <v>1962</v>
       </c>
       <c r="G86" s="25">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H86" s="26">
-        <v>6.7278287461773695E-2</v>
+        <v>6.7787971457696203E-2</v>
       </c>
       <c r="I86" s="25">
         <v>344</v>
       </c>
       <c r="J86" s="25">
-        <v>1605</v>
+        <v>1614</v>
       </c>
       <c r="K86" s="25">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L86" s="26">
-        <v>6.7278287461773695E-2</v>
+        <v>6.7787971457696203E-2</v>
       </c>
       <c r="M86" s="25">
         <v>344</v>
       </c>
       <c r="N86" s="25">
-        <v>1605</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -5083,10 +5074,10 @@
         <v>77</v>
       </c>
       <c r="B87" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C87" s="22" t="s">
         <v>170</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>171</v>
       </c>
       <c r="D87" s="23">
         <v>6</v>
@@ -5104,10 +5095,10 @@
         <v>3.1347447891022402E-2</v>
       </c>
       <c r="I87" s="25">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="J87" s="25">
-        <v>1309</v>
+        <v>1353</v>
       </c>
       <c r="K87" s="25">
         <v>191</v>
@@ -5116,10 +5107,10 @@
         <v>3.1347447891022402E-2</v>
       </c>
       <c r="M87" s="25">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="N87" s="25">
-        <v>1309</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -5127,10 +5118,10 @@
         <v>78</v>
       </c>
       <c r="B88" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C88" s="22" t="s">
         <v>172</v>
-      </c>
-      <c r="C88" s="22" t="s">
-        <v>173</v>
       </c>
       <c r="D88" s="23">
         <v>5</v>
@@ -5154,16 +5145,16 @@
         <v>318</v>
       </c>
       <c r="K88" s="25">
-        <v>4692</v>
+        <v>4696</v>
       </c>
       <c r="L88" s="26">
-        <v>1.51025505671503E-2</v>
+        <v>1.5115425716823901E-2</v>
       </c>
       <c r="M88" s="25">
         <v>2667</v>
       </c>
       <c r="N88" s="25">
-        <v>31870</v>
+        <v>31971</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -5171,10 +5162,10 @@
         <v>79</v>
       </c>
       <c r="B89" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="22" t="s">
         <v>174</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>175</v>
       </c>
       <c r="D89" s="23">
         <v>6</v>
@@ -5186,28 +5177,28 @@
         <v>154731</v>
       </c>
       <c r="G89" s="25">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="H89" s="26">
-        <v>1.0663268727784799E-2</v>
+        <v>1.06699751861042E-2</v>
       </c>
       <c r="I89" s="25">
-        <v>1720</v>
+        <v>1723</v>
       </c>
       <c r="J89" s="25">
-        <v>11242</v>
+        <v>11307</v>
       </c>
       <c r="K89" s="25">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="L89" s="26">
-        <v>1.09609580497767E-2</v>
+        <v>1.0967420878815399E-2</v>
       </c>
       <c r="M89" s="25">
-        <v>1768</v>
+        <v>1771</v>
       </c>
       <c r="N89" s="25">
-        <v>11969</v>
+        <v>12034</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -5215,10 +5206,10 @@
         <v>80</v>
       </c>
       <c r="B90" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="22" t="s">
         <v>176</v>
-      </c>
-      <c r="C90" s="22" t="s">
-        <v>177</v>
       </c>
       <c r="D90" s="23">
         <v>7</v>
@@ -5259,10 +5250,10 @@
         <v>81</v>
       </c>
       <c r="B91" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C91" s="22" t="s">
         <v>178</v>
-      </c>
-      <c r="C91" s="22" t="s">
-        <v>179</v>
       </c>
       <c r="D91" s="23">
         <v>6</v>
@@ -5283,7 +5274,7 @@
         <v>314</v>
       </c>
       <c r="J91" s="25">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="K91" s="25">
         <v>201</v>
@@ -5295,7 +5286,7 @@
         <v>314</v>
       </c>
       <c r="N91" s="25">
-        <v>1541</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -5303,10 +5294,10 @@
         <v>82</v>
       </c>
       <c r="B92" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" s="22" t="s">
         <v>180</v>
-      </c>
-      <c r="C92" s="22" t="s">
-        <v>181</v>
       </c>
       <c r="D92" s="23">
         <v>6</v>
@@ -5318,28 +5309,28 @@
         <v>141847</v>
       </c>
       <c r="G92" s="25">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="H92" s="26">
-        <v>1.8814939623701201E-2</v>
+        <v>1.88289806234203E-2</v>
       </c>
       <c r="I92" s="25">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="J92" s="25">
-        <v>10249</v>
+        <v>10327</v>
       </c>
       <c r="K92" s="25">
-        <v>2785</v>
+        <v>2788</v>
       </c>
       <c r="L92" s="26">
-        <v>1.9633830817712E-2</v>
+        <v>1.9654980366169101E-2</v>
       </c>
       <c r="M92" s="25">
         <v>2021</v>
       </c>
       <c r="N92" s="25">
-        <v>19242</v>
+        <v>19327</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -5347,10 +5338,10 @@
         <v>83</v>
       </c>
       <c r="B93" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="22" t="s">
         <v>182</v>
-      </c>
-      <c r="C93" s="22" t="s">
-        <v>183</v>
       </c>
       <c r="D93" s="23">
         <v>7</v>
@@ -5391,10 +5382,10 @@
         <v>84</v>
       </c>
       <c r="B94" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" s="22" t="s">
         <v>184</v>
-      </c>
-      <c r="C94" s="22" t="s">
-        <v>185</v>
       </c>
       <c r="D94" s="23">
         <v>7</v>
@@ -5406,28 +5397,28 @@
         <v>29929</v>
       </c>
       <c r="G94" s="25">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="H94" s="26">
-        <v>2.1684653680376802E-2</v>
+        <v>2.1718066089745702E-2</v>
       </c>
       <c r="I94" s="25">
         <v>676</v>
       </c>
       <c r="J94" s="25">
-        <v>3693</v>
+        <v>3698</v>
       </c>
       <c r="K94" s="25">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="L94" s="26">
-        <v>2.1684653680376802E-2</v>
+        <v>2.1718066089745702E-2</v>
       </c>
       <c r="M94" s="25">
         <v>676</v>
       </c>
       <c r="N94" s="25">
-        <v>3693</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -5435,10 +5426,10 @@
         <v>85</v>
       </c>
       <c r="B95" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C95" s="22" t="s">
         <v>186</v>
-      </c>
-      <c r="C95" s="22" t="s">
-        <v>187</v>
       </c>
       <c r="D95" s="23">
         <v>7</v>
@@ -5479,10 +5470,10 @@
         <v>86</v>
       </c>
       <c r="B96" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C96" s="22" t="s">
         <v>188</v>
-      </c>
-      <c r="C96" s="22" t="s">
-        <v>189</v>
       </c>
       <c r="D96" s="23">
         <v>7</v>
@@ -5494,28 +5485,28 @@
         <v>29930</v>
       </c>
       <c r="G96" s="25">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H96" s="26">
-        <v>1.44670898763782E-2</v>
+        <v>1.45005011693952E-2</v>
       </c>
       <c r="I96" s="25">
         <v>505</v>
       </c>
       <c r="J96" s="25">
-        <v>3057</v>
+        <v>3061</v>
       </c>
       <c r="K96" s="25">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="L96" s="26">
-        <v>1.44670898763782E-2</v>
+        <v>1.45005011693952E-2</v>
       </c>
       <c r="M96" s="25">
         <v>505</v>
       </c>
       <c r="N96" s="25">
-        <v>3057</v>
+        <v>3061</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -5523,10 +5514,10 @@
         <v>87</v>
       </c>
       <c r="B97" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="C97" s="22" t="s">
         <v>190</v>
-      </c>
-      <c r="C97" s="22" t="s">
-        <v>191</v>
       </c>
       <c r="D97" s="23">
         <v>7</v>
@@ -5567,10 +5558,10 @@
         <v>88</v>
       </c>
       <c r="B98" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C98" s="22" t="s">
         <v>192</v>
-      </c>
-      <c r="C98" s="22" t="s">
-        <v>193</v>
       </c>
       <c r="D98" s="23">
         <v>6</v>
@@ -5591,7 +5582,7 @@
         <v>442</v>
       </c>
       <c r="J98" s="25">
-        <v>1341</v>
+        <v>1346</v>
       </c>
       <c r="K98" s="25">
         <v>232</v>
@@ -5603,7 +5594,7 @@
         <v>442</v>
       </c>
       <c r="N98" s="25">
-        <v>1341</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
@@ -5611,10 +5602,10 @@
         <v>89</v>
       </c>
       <c r="B99" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99" s="22" t="s">
         <v>194</v>
-      </c>
-      <c r="C99" s="22" t="s">
-        <v>195</v>
       </c>
       <c r="D99" s="23">
         <v>6</v>
@@ -5626,28 +5617,28 @@
         <v>6236</v>
       </c>
       <c r="G99" s="25">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H99" s="26">
-        <v>3.6401539448364301E-2</v>
+        <v>3.6561898652982601E-2</v>
       </c>
       <c r="I99" s="25">
         <v>324</v>
       </c>
       <c r="J99" s="25">
-        <v>1542</v>
+        <v>1552</v>
       </c>
       <c r="K99" s="25">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L99" s="26">
-        <v>3.6401539448364301E-2</v>
+        <v>3.6561898652982601E-2</v>
       </c>
       <c r="M99" s="25">
         <v>324</v>
       </c>
       <c r="N99" s="25">
-        <v>1542</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -5655,10 +5646,10 @@
         <v>90</v>
       </c>
       <c r="B100" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" s="22" t="s">
         <v>196</v>
-      </c>
-      <c r="C100" s="22" t="s">
-        <v>197</v>
       </c>
       <c r="D100" s="23">
         <v>4</v>
@@ -5699,10 +5690,10 @@
         <v>91</v>
       </c>
       <c r="B101" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C101" s="22" t="s">
         <v>198</v>
-      </c>
-      <c r="C101" s="22" t="s">
-        <v>199</v>
       </c>
       <c r="D101" s="23">
         <v>2</v>
@@ -5726,16 +5717,16 @@
         <v>2997</v>
       </c>
       <c r="K101" s="25">
-        <v>10954</v>
+        <v>10957</v>
       </c>
       <c r="L101" s="26">
-        <v>2.1577731245555499E-2</v>
+        <v>2.15836407940069E-2</v>
       </c>
       <c r="M101" s="25">
         <v>4390</v>
       </c>
       <c r="N101" s="25">
-        <v>168990</v>
+        <v>169501</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -5743,10 +5734,10 @@
         <v>92</v>
       </c>
       <c r="B102" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C102" s="22" t="s">
         <v>200</v>
-      </c>
-      <c r="C102" s="22" t="s">
-        <v>201</v>
       </c>
       <c r="D102" s="23">
         <v>3</v>
@@ -5767,7 +5758,7 @@
         <v>1405</v>
       </c>
       <c r="J102" s="25">
-        <v>3732</v>
+        <v>3734</v>
       </c>
       <c r="K102" s="25">
         <v>404</v>
@@ -5779,7 +5770,7 @@
         <v>1877</v>
       </c>
       <c r="N102" s="25">
-        <v>5759</v>
+        <v>5762</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -5787,10 +5778,10 @@
         <v>93</v>
       </c>
       <c r="B103" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="C103" s="22" t="s">
         <v>202</v>
-      </c>
-      <c r="C103" s="22" t="s">
-        <v>203</v>
       </c>
       <c r="D103" s="23">
         <v>4</v>
@@ -5811,7 +5802,7 @@
         <v>858</v>
       </c>
       <c r="J103" s="25">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="K103" s="25">
         <v>271</v>
@@ -5823,7 +5814,7 @@
         <v>858</v>
       </c>
       <c r="N103" s="25">
-        <v>2027</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -5831,10 +5822,10 @@
         <v>94</v>
       </c>
       <c r="B104" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="C104" s="22" t="s">
         <v>204</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>205</v>
       </c>
       <c r="D104" s="23">
         <v>3</v>
@@ -5852,10 +5843,10 @@
         <v>9.2313383870112099E-3</v>
       </c>
       <c r="I104" s="25">
-        <v>3458</v>
+        <v>3470</v>
       </c>
       <c r="J104" s="25">
-        <v>15558</v>
+        <v>15677</v>
       </c>
       <c r="K104" s="25">
         <v>3143</v>
@@ -5864,10 +5855,10 @@
         <v>1.0196798536177E-2</v>
       </c>
       <c r="M104" s="25">
-        <v>3568</v>
+        <v>3577</v>
       </c>
       <c r="N104" s="25">
-        <v>18317</v>
+        <v>18437</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -5875,10 +5866,10 @@
         <v>95</v>
       </c>
       <c r="B105" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="C105" s="22" t="s">
         <v>206</v>
-      </c>
-      <c r="C105" s="22" t="s">
-        <v>207</v>
       </c>
       <c r="D105" s="23">
         <v>4</v>
@@ -5899,7 +5890,7 @@
         <v>412</v>
       </c>
       <c r="J105" s="25">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="K105" s="25">
         <v>199</v>
@@ -5911,7 +5902,7 @@
         <v>412</v>
       </c>
       <c r="N105" s="25">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -5919,10 +5910,10 @@
         <v>96</v>
       </c>
       <c r="B106" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="C106" s="22" t="s">
         <v>208</v>
-      </c>
-      <c r="C106" s="22" t="s">
-        <v>209</v>
       </c>
       <c r="D106" s="23">
         <v>4</v>
@@ -5963,10 +5954,10 @@
         <v>97</v>
       </c>
       <c r="B107" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C107" s="22" t="s">
         <v>210</v>
-      </c>
-      <c r="C107" s="22" t="s">
-        <v>211</v>
       </c>
       <c r="D107" s="23">
         <v>3</v>
@@ -5987,19 +5978,19 @@
         <v>2839</v>
       </c>
       <c r="J107" s="25">
-        <v>9347</v>
+        <v>9349</v>
       </c>
       <c r="K107" s="25">
-        <v>4859</v>
+        <v>4862</v>
       </c>
       <c r="L107" s="26">
-        <v>7.1925513647936506E-2</v>
+        <v>7.1969921250518001E-2</v>
       </c>
       <c r="M107" s="25">
         <v>4387</v>
       </c>
       <c r="N107" s="25">
-        <v>108211</v>
+        <v>108583</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -6007,10 +5998,10 @@
         <v>98</v>
       </c>
       <c r="B108" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="C108" s="22" t="s">
         <v>212</v>
-      </c>
-      <c r="C108" s="22" t="s">
-        <v>213</v>
       </c>
       <c r="D108" s="23">
         <v>4</v>
@@ -6031,7 +6022,7 @@
         <v>2621</v>
       </c>
       <c r="J108" s="25">
-        <v>10169</v>
+        <v>10172</v>
       </c>
       <c r="K108" s="25">
         <v>431</v>
@@ -6043,7 +6034,7 @@
         <v>2621</v>
       </c>
       <c r="N108" s="25">
-        <v>10169</v>
+        <v>10172</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -6051,10 +6042,10 @@
         <v>99</v>
       </c>
       <c r="B109" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C109" s="22" t="s">
         <v>214</v>
-      </c>
-      <c r="C109" s="22" t="s">
-        <v>215</v>
       </c>
       <c r="D109" s="23">
         <v>4</v>
@@ -6075,7 +6066,7 @@
         <v>4122</v>
       </c>
       <c r="J109" s="25">
-        <v>31479</v>
+        <v>31486</v>
       </c>
       <c r="K109" s="25">
         <v>1037</v>
@@ -6087,7 +6078,7 @@
         <v>4122</v>
       </c>
       <c r="N109" s="25">
-        <v>31479</v>
+        <v>31486</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -6095,10 +6086,10 @@
         <v>100</v>
       </c>
       <c r="B110" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="C110" s="22" t="s">
         <v>216</v>
-      </c>
-      <c r="C110" s="22" t="s">
-        <v>217</v>
       </c>
       <c r="D110" s="23">
         <v>4</v>
@@ -6110,28 +6101,28 @@
         <v>9106</v>
       </c>
       <c r="G110" s="25">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="H110" s="26">
-        <v>9.9275203162749806E-2</v>
+        <v>9.9385020865363494E-2</v>
       </c>
       <c r="I110" s="25">
         <v>3441</v>
       </c>
       <c r="J110" s="25">
-        <v>19727</v>
+        <v>20003</v>
       </c>
       <c r="K110" s="25">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="L110" s="26">
-        <v>9.9275203162749806E-2</v>
+        <v>9.9385020865363494E-2</v>
       </c>
       <c r="M110" s="25">
         <v>3441</v>
       </c>
       <c r="N110" s="25">
-        <v>19727</v>
+        <v>20003</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -6139,10 +6130,10 @@
         <v>101</v>
       </c>
       <c r="B111" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="C111" s="22" t="s">
         <v>218</v>
-      </c>
-      <c r="C111" s="22" t="s">
-        <v>219</v>
       </c>
       <c r="D111" s="23">
         <v>4</v>
@@ -6163,19 +6154,19 @@
         <v>2290</v>
       </c>
       <c r="J111" s="25">
-        <v>7576</v>
+        <v>7577</v>
       </c>
       <c r="K111" s="25">
-        <v>1317</v>
+        <v>1319</v>
       </c>
       <c r="L111" s="26">
-        <v>3.0771747003434598E-2</v>
+        <v>3.0818477067221101E-2</v>
       </c>
       <c r="M111" s="25">
         <v>2992</v>
       </c>
       <c r="N111" s="25">
-        <v>13381</v>
+        <v>13388</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
@@ -6183,10 +6174,10 @@
         <v>102</v>
       </c>
       <c r="B112" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C112" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C112" s="22" t="s">
-        <v>221</v>
       </c>
       <c r="D112" s="23">
         <v>5</v>
@@ -6198,28 +6189,28 @@
         <v>24452</v>
       </c>
       <c r="G112" s="25">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H112" s="26">
-        <v>1.02241125470309E-2</v>
+        <v>1.0265008997218999E-2</v>
       </c>
       <c r="I112" s="25">
         <v>470</v>
       </c>
       <c r="J112" s="25">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="K112" s="25">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L112" s="26">
-        <v>1.02241125470309E-2</v>
+        <v>1.0265008997218999E-2</v>
       </c>
       <c r="M112" s="25">
         <v>470</v>
       </c>
       <c r="N112" s="25">
-        <v>1151</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -6227,10 +6218,10 @@
         <v>103</v>
       </c>
       <c r="B113" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C113" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C113" s="22" t="s">
-        <v>223</v>
       </c>
       <c r="D113" s="23">
         <v>5</v>
@@ -6271,10 +6262,10 @@
         <v>104</v>
       </c>
       <c r="B114" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="C114" s="22" t="s">
         <v>224</v>
-      </c>
-      <c r="C114" s="22" t="s">
-        <v>225</v>
       </c>
       <c r="D114" s="23">
         <v>5</v>
@@ -6286,28 +6277,28 @@
         <v>4542</v>
       </c>
       <c r="G114" s="25">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H114" s="26">
-        <v>6.9793042712461395E-2</v>
+        <v>7.0013210039630097E-2</v>
       </c>
       <c r="I114" s="25">
         <v>880</v>
       </c>
       <c r="J114" s="25">
-        <v>3006</v>
+        <v>3007</v>
       </c>
       <c r="K114" s="25">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L114" s="26">
-        <v>6.9793042712461395E-2</v>
+        <v>7.0013210039630097E-2</v>
       </c>
       <c r="M114" s="25">
         <v>880</v>
       </c>
       <c r="N114" s="25">
-        <v>3006</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
@@ -6315,10 +6306,10 @@
         <v>105</v>
       </c>
       <c r="B115" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="C115" s="22" t="s">
         <v>226</v>
-      </c>
-      <c r="C115" s="22" t="s">
-        <v>227</v>
       </c>
       <c r="D115" s="23">
         <v>5</v>
@@ -6351,7 +6342,7 @@
         <v>353</v>
       </c>
       <c r="N115" s="25">
-        <v>1046</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
@@ -6359,10 +6350,10 @@
         <v>106</v>
       </c>
       <c r="B116" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="C116" s="22" t="s">
         <v>228</v>
-      </c>
-      <c r="C116" s="22" t="s">
-        <v>229</v>
       </c>
       <c r="D116" s="23">
         <v>6</v>
@@ -6383,7 +6374,7 @@
         <v>219</v>
       </c>
       <c r="J116" s="25">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="K116" s="25">
         <v>40</v>
@@ -6395,7 +6386,7 @@
         <v>219</v>
       </c>
       <c r="N116" s="25">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
@@ -6403,10 +6394,10 @@
         <v>107</v>
       </c>
       <c r="B117" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C117" s="22" t="s">
         <v>230</v>
-      </c>
-      <c r="C117" s="22" t="s">
-        <v>231</v>
       </c>
       <c r="D117" s="23">
         <v>6</v>
@@ -6427,7 +6418,7 @@
         <v>135</v>
       </c>
       <c r="J117" s="25">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K117" s="25">
         <v>39</v>
@@ -6439,7 +6430,7 @@
         <v>135</v>
       </c>
       <c r="N117" s="25">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
@@ -6447,10 +6438,10 @@
         <v>108</v>
       </c>
       <c r="B118" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C118" s="22" t="s">
         <v>232</v>
-      </c>
-      <c r="C118" s="22" t="s">
-        <v>233</v>
       </c>
       <c r="D118" s="23">
         <v>6</v>
@@ -6491,10 +6482,10 @@
         <v>109</v>
       </c>
       <c r="B119" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="C119" s="22" t="s">
         <v>234</v>
-      </c>
-      <c r="C119" s="22" t="s">
-        <v>235</v>
       </c>
       <c r="D119" s="23">
         <v>4</v>
@@ -6515,7 +6506,7 @@
         <v>3979</v>
       </c>
       <c r="J119" s="25">
-        <v>23591</v>
+        <v>23668</v>
       </c>
       <c r="K119" s="25">
         <v>781</v>
@@ -6527,7 +6518,7 @@
         <v>3990</v>
       </c>
       <c r="N119" s="25">
-        <v>24108</v>
+        <v>24185</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
@@ -6535,10 +6526,10 @@
         <v>110</v>
       </c>
       <c r="B120" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C120" s="22" t="s">
         <v>236</v>
-      </c>
-      <c r="C120" s="22" t="s">
-        <v>237</v>
       </c>
       <c r="D120" s="23">
         <v>5</v>
@@ -6579,10 +6570,10 @@
         <v>111</v>
       </c>
       <c r="B121" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C121" s="22" t="s">
         <v>238</v>
-      </c>
-      <c r="C121" s="22" t="s">
-        <v>239</v>
       </c>
       <c r="D121" s="23">
         <v>3</v>
@@ -6623,10 +6614,10 @@
         <v>112</v>
       </c>
       <c r="B122" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="C122" s="22" t="s">
         <v>240</v>
-      </c>
-      <c r="C122" s="22" t="s">
-        <v>241</v>
       </c>
       <c r="D122" s="23">
         <v>4</v>
@@ -6667,10 +6658,10 @@
         <v>113</v>
       </c>
       <c r="B123" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="C123" s="22" t="s">
         <v>242</v>
-      </c>
-      <c r="C123" s="22" t="s">
-        <v>243</v>
       </c>
       <c r="D123" s="23">
         <v>3</v>
@@ -6691,7 +6682,7 @@
         <v>225</v>
       </c>
       <c r="J123" s="25">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="K123" s="25">
         <v>291</v>
@@ -6703,7 +6694,7 @@
         <v>882</v>
       </c>
       <c r="N123" s="25">
-        <v>2246</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
@@ -6711,10 +6702,10 @@
         <v>114</v>
       </c>
       <c r="B124" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="C124" s="22" t="s">
         <v>244</v>
-      </c>
-      <c r="C124" s="22" t="s">
-        <v>245</v>
       </c>
       <c r="D124" s="23">
         <v>4</v>
@@ -6735,7 +6726,7 @@
         <v>727</v>
       </c>
       <c r="J124" s="25">
-        <v>1772</v>
+        <v>1779</v>
       </c>
       <c r="K124" s="25">
         <v>211</v>
@@ -6747,7 +6738,7 @@
         <v>727</v>
       </c>
       <c r="N124" s="25">
-        <v>1772</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
@@ -6755,10 +6746,10 @@
         <v>115</v>
       </c>
       <c r="B125" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="C125" s="22" t="s">
         <v>246</v>
-      </c>
-      <c r="C125" s="22" t="s">
-        <v>247</v>
       </c>
       <c r="D125" s="23">
         <v>4</v>
@@ -6799,10 +6790,10 @@
         <v>116</v>
       </c>
       <c r="B126" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="C126" s="22" t="s">
         <v>248</v>
-      </c>
-      <c r="C126" s="22" t="s">
-        <v>249</v>
       </c>
       <c r="D126" s="23">
         <v>4</v>
@@ -6843,10 +6834,10 @@
         <v>117</v>
       </c>
       <c r="B127" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="C127" s="22" t="s">
         <v>250</v>
-      </c>
-      <c r="C127" s="22" t="s">
-        <v>251</v>
       </c>
       <c r="D127" s="23">
         <v>3</v>
@@ -6879,7 +6870,7 @@
         <v>2830</v>
       </c>
       <c r="N127" s="25">
-        <v>18494</v>
+        <v>18499</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
@@ -6887,10 +6878,10 @@
         <v>118</v>
       </c>
       <c r="B128" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="C128" s="22" t="s">
         <v>252</v>
-      </c>
-      <c r="C128" s="22" t="s">
-        <v>253</v>
       </c>
       <c r="D128" s="23">
         <v>4</v>
@@ -6931,10 +6922,10 @@
         <v>119</v>
       </c>
       <c r="B129" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="C129" s="22" t="s">
         <v>254</v>
-      </c>
-      <c r="C129" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="D129" s="23">
         <v>4</v>
@@ -6975,10 +6966,10 @@
         <v>120</v>
       </c>
       <c r="B130" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C130" s="22" t="s">
         <v>256</v>
-      </c>
-      <c r="C130" s="22" t="s">
-        <v>257</v>
       </c>
       <c r="D130" s="23">
         <v>4</v>
@@ -7019,10 +7010,10 @@
         <v>121</v>
       </c>
       <c r="B131" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="C131" s="22" t="s">
         <v>258</v>
-      </c>
-      <c r="C131" s="22" t="s">
-        <v>259</v>
       </c>
       <c r="D131" s="23">
         <v>4</v>
@@ -7063,10 +7054,10 @@
         <v>122</v>
       </c>
       <c r="B132" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="C132" s="22" t="s">
         <v>260</v>
-      </c>
-      <c r="C132" s="22" t="s">
-        <v>261</v>
       </c>
       <c r="D132" s="23">
         <v>4</v>
@@ -7087,7 +7078,7 @@
         <v>1520</v>
       </c>
       <c r="J132" s="25">
-        <v>6300</v>
+        <v>6305</v>
       </c>
       <c r="K132" s="25">
         <v>37</v>
@@ -7099,7 +7090,7 @@
         <v>1520</v>
       </c>
       <c r="N132" s="25">
-        <v>6300</v>
+        <v>6305</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
@@ -7107,10 +7098,10 @@
         <v>123</v>
       </c>
       <c r="B133" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C133" s="22" t="s">
         <v>262</v>
-      </c>
-      <c r="C133" s="22" t="s">
-        <v>263</v>
       </c>
       <c r="D133" s="23">
         <v>3</v>
@@ -7151,10 +7142,10 @@
         <v>124</v>
       </c>
       <c r="B134" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="C134" s="22" t="s">
         <v>264</v>
-      </c>
-      <c r="C134" s="22" t="s">
-        <v>265</v>
       </c>
       <c r="D134" s="23">
         <v>3</v>
@@ -7175,7 +7166,7 @@
         <v>2450</v>
       </c>
       <c r="J134" s="25">
-        <v>9880</v>
+        <v>9882</v>
       </c>
       <c r="K134" s="25">
         <v>1110</v>
@@ -7187,7 +7178,7 @@
         <v>2660</v>
       </c>
       <c r="N134" s="25">
-        <v>11375</v>
+        <v>11377</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
@@ -7195,10 +7186,10 @@
         <v>125</v>
       </c>
       <c r="B135" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="C135" s="22" t="s">
         <v>266</v>
-      </c>
-      <c r="C135" s="22" t="s">
-        <v>267</v>
       </c>
       <c r="D135" s="23">
         <v>4</v>
@@ -7239,10 +7230,10 @@
         <v>126</v>
       </c>
       <c r="B136" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="C136" s="22" t="s">
         <v>268</v>
-      </c>
-      <c r="C136" s="22" t="s">
-        <v>269</v>
       </c>
       <c r="D136" s="23">
         <v>4</v>
@@ -7283,10 +7274,10 @@
         <v>127</v>
       </c>
       <c r="B137" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="C137" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="C137" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="D137" s="23">
         <v>3</v>
@@ -7327,13 +7318,13 @@
         <v>128</v>
       </c>
       <c r="B138" s="32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C138" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D138" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E138" s="24">
         <v>0</v>
@@ -7351,7 +7342,7 @@
         <v>1088</v>
       </c>
       <c r="J138" s="25">
-        <v>2468</v>
+        <v>2475</v>
       </c>
       <c r="K138" s="25">
         <v>685</v>
@@ -7363,7 +7354,7 @@
         <v>1088</v>
       </c>
       <c r="N138" s="25">
-        <v>2468</v>
+        <v>2475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected version of full corpus data to remove null-span mentions, and corresponding stats and descriptions. Added ST21pv subset corpus.
</commit_message>
<xml_diff>
--- a/full/stats/TypeMentionStats.xlsx
+++ b/full/stats/TypeMentionStats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunilmohan/Home/Projects/MedMentions/full/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12160B0D-12D7-444A-A29D-89D8008E303E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86F01F5-104C-EF40-8C08-16DF7D7C16EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40080" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{900A78CF-1263-6D42-B34D-1DC694662144}"/>
+    <workbookView xWindow="10520" yWindow="460" windowWidth="27640" windowHeight="25680" xr2:uid="{900A78CF-1263-6D42-B34D-1DC694662144}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -940,7 +940,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1138,11 +1138,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1230,9 +1254,27 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1550,7 +1592,7 @@
   <dimension ref="A1:N138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1617,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>34728</v>
+        <v>34724</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -1626,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>352594</v>
+        <v>352496</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1668,13 +1710,13 @@
         <v>277</v>
       </c>
       <c r="F9" s="43"/>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="47" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36" t="s">
+      <c r="J9" s="48"/>
+      <c r="K9" s="41" t="s">
         <v>6</v>
       </c>
       <c r="L9" s="36"/>
@@ -1697,10 +1739,10 @@
       <c r="E10" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="49" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="12" t="s">
@@ -1709,10 +1751,10 @@
       <c r="I10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="L10" s="12" t="s">
@@ -1741,10 +1783,10 @@
       <c r="E11" s="18">
         <v>185</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="45">
         <v>740300</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="50">
         <v>16</v>
       </c>
       <c r="H11" s="20">
@@ -1753,10 +1795,10 @@
       <c r="I11" s="19">
         <v>146</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="51">
         <v>292</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="18">
         <v>11539</v>
       </c>
       <c r="L11" s="20">
@@ -1766,7 +1808,7 @@
         <v>4380</v>
       </c>
       <c r="N11" s="19">
-        <v>99600</v>
+        <v>99567</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1785,10 +1827,10 @@
       <c r="E12" s="24">
         <v>420</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="46">
         <v>399121</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="52">
         <v>152</v>
       </c>
       <c r="H12" s="26">
@@ -1797,10 +1839,10 @@
       <c r="I12" s="25">
         <v>2615</v>
       </c>
-      <c r="J12" s="25">
-        <v>7254</v>
-      </c>
-      <c r="K12" s="25">
+      <c r="J12" s="53">
+        <v>7253</v>
+      </c>
+      <c r="K12" s="24">
         <v>5128</v>
       </c>
       <c r="L12" s="26">
@@ -1810,7 +1852,7 @@
         <v>4283</v>
       </c>
       <c r="N12" s="25">
-        <v>48531</v>
+        <v>48520</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1829,10 +1871,10 @@
       <c r="E13" s="24">
         <v>84</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="46">
         <v>1865</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="52">
         <v>23</v>
       </c>
       <c r="H13" s="26">
@@ -1841,10 +1883,10 @@
       <c r="I13" s="25">
         <v>191</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="53">
         <v>447</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="24">
         <v>343</v>
       </c>
       <c r="L13" s="26">
@@ -1873,10 +1915,10 @@
       <c r="E14" s="24">
         <v>924</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="46">
         <v>924</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="52">
         <v>171</v>
       </c>
       <c r="H14" s="26">
@@ -1885,10 +1927,10 @@
       <c r="I14" s="25">
         <v>382</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="53">
         <v>982</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="24">
         <v>171</v>
       </c>
       <c r="L14" s="26">
@@ -1917,10 +1959,10 @@
       <c r="E15" s="24">
         <v>857</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="46">
         <v>857</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="52">
         <v>149</v>
       </c>
       <c r="H15" s="26">
@@ -1929,10 +1971,10 @@
       <c r="I15" s="25">
         <v>352</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="53">
         <v>1012</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="24">
         <v>149</v>
       </c>
       <c r="L15" s="26">
@@ -1961,10 +2003,10 @@
       <c r="E16" s="24">
         <v>808</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="46">
         <v>808</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="52">
         <v>71</v>
       </c>
       <c r="H16" s="26">
@@ -1973,10 +2015,10 @@
       <c r="I16" s="25">
         <v>218</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="53">
         <v>863</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="24">
         <v>71</v>
       </c>
       <c r="L16" s="26">
@@ -2005,10 +2047,10 @@
       <c r="E17" s="24">
         <v>739</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="46">
         <v>395894</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="52">
         <v>130</v>
       </c>
       <c r="H17" s="26">
@@ -2017,10 +2059,10 @@
       <c r="I17" s="25">
         <v>465</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="53">
         <v>891</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="24">
         <v>4527</v>
       </c>
       <c r="L17" s="26">
@@ -2030,7 +2072,7 @@
         <v>4142</v>
       </c>
       <c r="N17" s="25">
-        <v>37694</v>
+        <v>37684</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -2049,10 +2091,10 @@
       <c r="E18" s="24">
         <v>24725</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="46">
         <v>390903</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="52">
         <v>626</v>
       </c>
       <c r="H18" s="26">
@@ -2061,10 +2103,10 @@
       <c r="I18" s="25">
         <v>1840</v>
       </c>
-      <c r="J18" s="25">
-        <v>5683</v>
-      </c>
-      <c r="K18" s="25">
+      <c r="J18" s="53">
+        <v>5681</v>
+      </c>
+      <c r="K18" s="24">
         <v>3760</v>
       </c>
       <c r="L18" s="26">
@@ -2074,7 +2116,7 @@
         <v>3593</v>
       </c>
       <c r="N18" s="25">
-        <v>26310</v>
+        <v>26300</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -2093,10 +2135,10 @@
       <c r="E19" s="24">
         <v>31562</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="46">
         <v>31562</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="52">
         <v>908</v>
       </c>
       <c r="H19" s="26">
@@ -2105,10 +2147,10 @@
       <c r="I19" s="25">
         <v>1546</v>
       </c>
-      <c r="J19" s="25">
-        <v>5111</v>
-      </c>
-      <c r="K19" s="25">
+      <c r="J19" s="53">
+        <v>5107</v>
+      </c>
+      <c r="K19" s="24">
         <v>908</v>
       </c>
       <c r="L19" s="26">
@@ -2118,7 +2160,7 @@
         <v>1546</v>
       </c>
       <c r="N19" s="25">
-        <v>5111</v>
+        <v>5107</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -2137,10 +2179,10 @@
       <c r="E20" s="24">
         <v>48254</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="46">
         <v>48254</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="52">
         <v>608</v>
       </c>
       <c r="H20" s="26">
@@ -2149,10 +2191,10 @@
       <c r="I20" s="25">
         <v>1043</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="53">
         <v>4083</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="24">
         <v>608</v>
       </c>
       <c r="L20" s="26">
@@ -2181,10 +2223,10 @@
       <c r="E21" s="24">
         <v>286362</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="46">
         <v>286362</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="52">
         <v>1618</v>
       </c>
       <c r="H21" s="26">
@@ -2193,10 +2235,10 @@
       <c r="I21" s="25">
         <v>2145</v>
       </c>
-      <c r="J21" s="25">
-        <v>11433</v>
-      </c>
-      <c r="K21" s="25">
+      <c r="J21" s="53">
+        <v>11429</v>
+      </c>
+      <c r="K21" s="24">
         <v>1618</v>
       </c>
       <c r="L21" s="26">
@@ -2206,7 +2248,7 @@
         <v>2145</v>
       </c>
       <c r="N21" s="25">
-        <v>11433</v>
+        <v>11429</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -2225,10 +2267,10 @@
       <c r="E22" s="24">
         <v>1284</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="46">
         <v>1598</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="52">
         <v>413</v>
       </c>
       <c r="H22" s="26">
@@ -2237,10 +2279,10 @@
       <c r="I22" s="25">
         <v>3007</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="53">
         <v>8859</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="24">
         <v>538</v>
       </c>
       <c r="L22" s="26">
@@ -2269,10 +2311,10 @@
       <c r="E23" s="24">
         <v>314</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="46">
         <v>314</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="52">
         <v>125</v>
       </c>
       <c r="H23" s="26">
@@ -2281,10 +2323,10 @@
       <c r="I23" s="25">
         <v>516</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J23" s="53">
         <v>1106</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="24">
         <v>125</v>
       </c>
       <c r="L23" s="26">
@@ -2313,10 +2355,10 @@
       <c r="E24" s="24">
         <v>516</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="46">
         <v>516</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="52">
         <v>61</v>
       </c>
       <c r="H24" s="26">
@@ -2325,10 +2367,10 @@
       <c r="I24" s="25">
         <v>94</v>
       </c>
-      <c r="J24" s="25">
+      <c r="J24" s="53">
         <v>188</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="24">
         <v>61</v>
       </c>
       <c r="L24" s="26">
@@ -2357,10 +2399,10 @@
       <c r="E25" s="24">
         <v>2241</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="46">
         <v>2241</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="52">
         <v>74</v>
       </c>
       <c r="H25" s="26">
@@ -2369,10 +2411,10 @@
       <c r="I25" s="25">
         <v>172</v>
       </c>
-      <c r="J25" s="25">
+      <c r="J25" s="53">
         <v>554</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="24">
         <v>74</v>
       </c>
       <c r="L25" s="26">
@@ -2401,10 +2443,10 @@
       <c r="E26" s="24">
         <v>155</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="46">
         <v>155</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="52">
         <v>37</v>
       </c>
       <c r="H26" s="26">
@@ -2413,10 +2455,10 @@
       <c r="I26" s="25">
         <v>125</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="53">
         <v>288</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="24">
         <v>37</v>
       </c>
       <c r="L26" s="26">
@@ -2445,10 +2487,10 @@
       <c r="E27" s="24">
         <v>1615</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="46">
         <v>340994</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="52">
         <v>154</v>
       </c>
       <c r="H27" s="26">
@@ -2457,10 +2499,10 @@
       <c r="I27" s="25">
         <v>900</v>
       </c>
-      <c r="J27" s="25">
-        <v>2035</v>
-      </c>
-      <c r="K27" s="25">
+      <c r="J27" s="53">
+        <v>2034</v>
+      </c>
+      <c r="K27" s="24">
         <v>6395</v>
       </c>
       <c r="L27" s="26">
@@ -2470,7 +2512,7 @@
         <v>4206</v>
       </c>
       <c r="N27" s="25">
-        <v>50777</v>
+        <v>50755</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -2489,10 +2531,10 @@
       <c r="E28" s="24">
         <v>104583</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="46">
         <v>104583</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="52">
         <v>274</v>
       </c>
       <c r="H28" s="26">
@@ -2501,10 +2543,10 @@
       <c r="I28" s="25">
         <v>521</v>
       </c>
-      <c r="J28" s="25">
-        <v>1896</v>
-      </c>
-      <c r="K28" s="25">
+      <c r="J28" s="53">
+        <v>1895</v>
+      </c>
+      <c r="K28" s="24">
         <v>274</v>
       </c>
       <c r="L28" s="26">
@@ -2514,7 +2556,7 @@
         <v>521</v>
       </c>
       <c r="N28" s="25">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -2533,10 +2575,10 @@
       <c r="E29" s="24">
         <v>560</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="46">
         <v>628</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="52">
         <v>48</v>
       </c>
       <c r="H29" s="26">
@@ -2545,10 +2587,10 @@
       <c r="I29" s="25">
         <v>173</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="53">
         <v>295</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="24">
         <v>75</v>
       </c>
       <c r="L29" s="26">
@@ -2577,10 +2619,10 @@
       <c r="E30" s="24">
         <v>68</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="46">
         <v>68</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="52">
         <v>27</v>
       </c>
       <c r="H30" s="26">
@@ -2589,10 +2631,10 @@
       <c r="I30" s="25">
         <v>62</v>
       </c>
-      <c r="J30" s="25">
+      <c r="J30" s="53">
         <v>190</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="24">
         <v>27</v>
       </c>
       <c r="L30" s="26">
@@ -2621,10 +2663,10 @@
       <c r="E31" s="24">
         <v>749</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="46">
         <v>234172</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="52">
         <v>306</v>
       </c>
       <c r="H31" s="26">
@@ -2633,10 +2675,10 @@
       <c r="I31" s="25">
         <v>956</v>
       </c>
-      <c r="J31" s="25">
-        <v>2834</v>
-      </c>
-      <c r="K31" s="25">
+      <c r="J31" s="53">
+        <v>2831</v>
+      </c>
+      <c r="K31" s="24">
         <v>5893</v>
       </c>
       <c r="L31" s="26">
@@ -2646,7 +2688,7 @@
         <v>4115</v>
       </c>
       <c r="N31" s="25">
-        <v>46365</v>
+        <v>46345</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -2665,10 +2707,10 @@
       <c r="E32" s="24">
         <v>1624</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="46">
         <v>233423</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="52">
         <v>78</v>
       </c>
       <c r="H32" s="26">
@@ -2677,10 +2719,10 @@
       <c r="I32" s="25">
         <v>489</v>
       </c>
-      <c r="J32" s="25">
+      <c r="J32" s="53">
         <v>946</v>
       </c>
-      <c r="K32" s="25">
+      <c r="K32" s="24">
         <v>5587</v>
       </c>
       <c r="L32" s="26">
@@ -2690,7 +2732,7 @@
         <v>3955</v>
       </c>
       <c r="N32" s="25">
-        <v>43531</v>
+        <v>43514</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -2709,10 +2751,10 @@
       <c r="E33" s="24">
         <v>2368</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="46">
         <v>65441</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="52">
         <v>176</v>
       </c>
       <c r="H33" s="26">
@@ -2721,10 +2763,10 @@
       <c r="I33" s="25">
         <v>581</v>
       </c>
-      <c r="J33" s="25">
-        <v>1312</v>
-      </c>
-      <c r="K33" s="25">
+      <c r="J33" s="53">
+        <v>1311</v>
+      </c>
+      <c r="K33" s="24">
         <v>2419</v>
       </c>
       <c r="L33" s="26">
@@ -2734,7 +2776,7 @@
         <v>2984</v>
       </c>
       <c r="N33" s="25">
-        <v>18962</v>
+        <v>18956</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -2753,10 +2795,10 @@
       <c r="E34" s="24">
         <v>4863</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="46">
         <v>6278</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="52">
         <v>313</v>
       </c>
       <c r="H34" s="26">
@@ -2765,10 +2807,10 @@
       <c r="I34" s="25">
         <v>1032</v>
       </c>
-      <c r="J34" s="25">
-        <v>2715</v>
-      </c>
-      <c r="K34" s="25">
+      <c r="J34" s="53">
+        <v>2713</v>
+      </c>
+      <c r="K34" s="24">
         <v>650</v>
       </c>
       <c r="L34" s="26">
@@ -2778,7 +2820,7 @@
         <v>1645</v>
       </c>
       <c r="N34" s="25">
-        <v>5950</v>
+        <v>5948</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -2797,10 +2839,10 @@
       <c r="E35" s="24">
         <v>1415</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="46">
         <v>1415</v>
       </c>
-      <c r="G35" s="25">
+      <c r="G35" s="52">
         <v>337</v>
       </c>
       <c r="H35" s="26">
@@ -2809,10 +2851,10 @@
       <c r="I35" s="25">
         <v>838</v>
       </c>
-      <c r="J35" s="25">
+      <c r="J35" s="53">
         <v>3235</v>
       </c>
-      <c r="K35" s="25">
+      <c r="K35" s="24">
         <v>337</v>
       </c>
       <c r="L35" s="26">
@@ -2841,10 +2883,10 @@
       <c r="E36" s="24">
         <v>4654</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="46">
         <v>4654</v>
       </c>
-      <c r="G36" s="25">
+      <c r="G36" s="52">
         <v>320</v>
       </c>
       <c r="H36" s="26">
@@ -2853,10 +2895,10 @@
       <c r="I36" s="25">
         <v>611</v>
       </c>
-      <c r="J36" s="25">
+      <c r="J36" s="53">
         <v>1699</v>
       </c>
-      <c r="K36" s="25">
+      <c r="K36" s="24">
         <v>320</v>
       </c>
       <c r="L36" s="26">
@@ -2885,10 +2927,10 @@
       <c r="E37" s="24">
         <v>17924</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="46">
         <v>17924</v>
       </c>
-      <c r="G37" s="25">
+      <c r="G37" s="52">
         <v>491</v>
       </c>
       <c r="H37" s="26">
@@ -2897,10 +2939,10 @@
       <c r="I37" s="25">
         <v>809</v>
       </c>
-      <c r="J37" s="25">
-        <v>3090</v>
-      </c>
-      <c r="K37" s="25">
+      <c r="J37" s="53">
+        <v>3089</v>
+      </c>
+      <c r="K37" s="24">
         <v>491</v>
       </c>
       <c r="L37" s="26">
@@ -2910,7 +2952,7 @@
         <v>809</v>
       </c>
       <c r="N37" s="25">
-        <v>3090</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -2929,10 +2971,10 @@
       <c r="E38" s="24">
         <v>29590</v>
       </c>
-      <c r="F38" s="25">
+      <c r="F38" s="46">
         <v>34217</v>
       </c>
-      <c r="G38" s="25">
+      <c r="G38" s="52">
         <v>578</v>
       </c>
       <c r="H38" s="26">
@@ -2941,10 +2983,10 @@
       <c r="I38" s="25">
         <v>1025</v>
       </c>
-      <c r="J38" s="25">
+      <c r="J38" s="53">
         <v>3471</v>
       </c>
-      <c r="K38" s="25">
+      <c r="K38" s="24">
         <v>782</v>
       </c>
       <c r="L38" s="26">
@@ -2954,7 +2996,7 @@
         <v>1420</v>
       </c>
       <c r="N38" s="25">
-        <v>6911</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -2973,10 +3015,10 @@
       <c r="E39" s="24">
         <v>4627</v>
       </c>
-      <c r="F39" s="25">
+      <c r="F39" s="46">
         <v>4627</v>
       </c>
-      <c r="G39" s="25">
+      <c r="G39" s="52">
         <v>204</v>
       </c>
       <c r="H39" s="26">
@@ -2985,10 +3027,10 @@
       <c r="I39" s="25">
         <v>931</v>
       </c>
-      <c r="J39" s="25">
-        <v>3440</v>
-      </c>
-      <c r="K39" s="25">
+      <c r="J39" s="53">
+        <v>3438</v>
+      </c>
+      <c r="K39" s="24">
         <v>204</v>
       </c>
       <c r="L39" s="26">
@@ -2998,7 +3040,7 @@
         <v>931</v>
       </c>
       <c r="N39" s="25">
-        <v>3440</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -3017,10 +3059,10 @@
       <c r="E40" s="24">
         <v>24341</v>
       </c>
-      <c r="F40" s="25">
+      <c r="F40" s="46">
         <v>166358</v>
       </c>
-      <c r="G40" s="25">
+      <c r="G40" s="52">
         <v>443</v>
       </c>
       <c r="H40" s="26">
@@ -3029,10 +3071,10 @@
       <c r="I40" s="25">
         <v>1311</v>
       </c>
-      <c r="J40" s="25">
-        <v>3964</v>
-      </c>
-      <c r="K40" s="25">
+      <c r="J40" s="53">
+        <v>3962</v>
+      </c>
+      <c r="K40" s="24">
         <v>3090</v>
       </c>
       <c r="L40" s="26">
@@ -3042,7 +3084,7 @@
         <v>2941</v>
       </c>
       <c r="N40" s="25">
-        <v>23623</v>
+        <v>23612</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -3061,10 +3103,10 @@
       <c r="E41" s="24">
         <v>95108</v>
       </c>
-      <c r="F41" s="25">
+      <c r="F41" s="46">
         <v>139732</v>
       </c>
-      <c r="G41" s="25">
+      <c r="G41" s="52">
         <v>1677</v>
       </c>
       <c r="H41" s="26">
@@ -3073,10 +3115,10 @@
       <c r="I41" s="25">
         <v>1925</v>
       </c>
-      <c r="J41" s="25">
-        <v>11754</v>
-      </c>
-      <c r="K41" s="25">
+      <c r="J41" s="53">
+        <v>11750</v>
+      </c>
+      <c r="K41" s="24">
         <v>2524</v>
       </c>
       <c r="L41" s="26">
@@ -3086,7 +3128,7 @@
         <v>2574</v>
       </c>
       <c r="N41" s="25">
-        <v>18777</v>
+        <v>18769</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -3105,10 +3147,10 @@
       <c r="E42" s="24">
         <v>7369</v>
       </c>
-      <c r="F42" s="25">
+      <c r="F42" s="46">
         <v>7369</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="52">
         <v>243</v>
       </c>
       <c r="H42" s="26">
@@ -3117,10 +3159,10 @@
       <c r="I42" s="25">
         <v>400</v>
       </c>
-      <c r="J42" s="25">
+      <c r="J42" s="53">
         <v>2284</v>
       </c>
-      <c r="K42" s="25">
+      <c r="K42" s="24">
         <v>243</v>
       </c>
       <c r="L42" s="26">
@@ -3149,10 +3191,10 @@
       <c r="E43" s="24">
         <v>37255</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F43" s="46">
         <v>37255</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="52">
         <v>604</v>
       </c>
       <c r="H43" s="26">
@@ -3161,10 +3203,10 @@
       <c r="I43" s="25">
         <v>705</v>
       </c>
-      <c r="J43" s="25">
-        <v>4739</v>
-      </c>
-      <c r="K43" s="25">
+      <c r="J43" s="53">
+        <v>4735</v>
+      </c>
+      <c r="K43" s="24">
         <v>604</v>
       </c>
       <c r="L43" s="26">
@@ -3174,7 +3216,7 @@
         <v>705</v>
       </c>
       <c r="N43" s="25">
-        <v>4739</v>
+        <v>4735</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -3193,32 +3235,32 @@
       <c r="E44" s="24">
         <v>2182</v>
       </c>
-      <c r="F44" s="25">
+      <c r="F44" s="46">
         <v>2182</v>
       </c>
-      <c r="G44" s="25">
+      <c r="G44" s="52">
         <v>104</v>
       </c>
       <c r="H44" s="26">
         <v>4.7662694775435298E-2</v>
       </c>
       <c r="I44" s="25">
-        <v>284</v>
-      </c>
-      <c r="J44" s="25">
-        <v>595</v>
-      </c>
-      <c r="K44" s="25">
+        <v>283</v>
+      </c>
+      <c r="J44" s="53">
+        <v>594</v>
+      </c>
+      <c r="K44" s="24">
         <v>104</v>
       </c>
       <c r="L44" s="26">
         <v>4.7662694775435298E-2</v>
       </c>
       <c r="M44" s="25">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N44" s="25">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -3237,10 +3279,10 @@
       <c r="E45" s="24">
         <v>129</v>
       </c>
-      <c r="F45" s="25">
+      <c r="F45" s="46">
         <v>129</v>
       </c>
-      <c r="G45" s="25">
+      <c r="G45" s="52">
         <v>20</v>
       </c>
       <c r="H45" s="26">
@@ -3249,10 +3291,10 @@
       <c r="I45" s="25">
         <v>148</v>
       </c>
-      <c r="J45" s="25">
+      <c r="J45" s="53">
         <v>288</v>
       </c>
-      <c r="K45" s="25">
+      <c r="K45" s="24">
         <v>20</v>
       </c>
       <c r="L45" s="26">
@@ -3281,10 +3323,10 @@
       <c r="E46" s="24">
         <v>23</v>
       </c>
-      <c r="F46" s="25">
+      <c r="F46" s="46">
         <v>2531566</v>
       </c>
-      <c r="G46" s="25">
+      <c r="G46" s="52">
         <v>6</v>
       </c>
       <c r="H46" s="26">
@@ -3293,20 +3335,20 @@
       <c r="I46" s="25">
         <v>81</v>
       </c>
-      <c r="J46" s="25">
+      <c r="J46" s="53">
         <v>109</v>
       </c>
-      <c r="K46" s="25">
-        <v>22551</v>
+      <c r="K46" s="24">
+        <v>22547</v>
       </c>
       <c r="L46" s="26">
-        <v>8.9079249760819906E-3</v>
+        <v>8.9063449264210302E-3</v>
       </c>
       <c r="M46" s="25">
         <v>4392</v>
       </c>
       <c r="N46" s="25">
-        <v>250857</v>
+        <v>250794</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -3325,10 +3367,10 @@
       <c r="E47" s="24">
         <v>42</v>
       </c>
-      <c r="F47" s="25">
+      <c r="F47" s="46">
         <v>2025030</v>
       </c>
-      <c r="G47" s="25">
+      <c r="G47" s="52">
         <v>6</v>
       </c>
       <c r="H47" s="26">
@@ -3337,20 +3379,20 @@
       <c r="I47" s="25">
         <v>29</v>
       </c>
-      <c r="J47" s="25">
+      <c r="J47" s="53">
         <v>79</v>
       </c>
-      <c r="K47" s="25">
-        <v>11727</v>
+      <c r="K47" s="24">
+        <v>11725</v>
       </c>
       <c r="L47" s="26">
-        <v>5.79102531814343E-3</v>
+        <v>5.7900376784541397E-3</v>
       </c>
       <c r="M47" s="25">
         <v>4013</v>
       </c>
       <c r="N47" s="25">
-        <v>82788</v>
+        <v>82759</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -3369,10 +3411,10 @@
       <c r="E48" s="24">
         <v>118</v>
       </c>
-      <c r="F48" s="25">
+      <c r="F48" s="46">
         <v>1180613</v>
       </c>
-      <c r="G48" s="25">
+      <c r="G48" s="52">
         <v>41</v>
       </c>
       <c r="H48" s="26">
@@ -3381,10 +3423,10 @@
       <c r="I48" s="25">
         <v>377</v>
       </c>
-      <c r="J48" s="25">
+      <c r="J48" s="53">
         <v>1038</v>
       </c>
-      <c r="K48" s="25">
+      <c r="K48" s="24">
         <v>1803</v>
       </c>
       <c r="L48" s="26">
@@ -3394,7 +3436,7 @@
         <v>1727</v>
       </c>
       <c r="N48" s="25">
-        <v>12855</v>
+        <v>12853</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3413,10 +3455,10 @@
       <c r="E49" s="24">
         <v>18128</v>
       </c>
-      <c r="F49" s="25">
+      <c r="F49" s="46">
         <v>18128</v>
       </c>
-      <c r="G49" s="25">
+      <c r="G49" s="52">
         <v>131</v>
       </c>
       <c r="H49" s="26">
@@ -3425,10 +3467,10 @@
       <c r="I49" s="25">
         <v>174</v>
       </c>
-      <c r="J49" s="25">
+      <c r="J49" s="53">
         <v>1105</v>
       </c>
-      <c r="K49" s="25">
+      <c r="K49" s="24">
         <v>131</v>
       </c>
       <c r="L49" s="26">
@@ -3457,10 +3499,10 @@
       <c r="E50" s="24">
         <v>350363</v>
       </c>
-      <c r="F50" s="25">
+      <c r="F50" s="46">
         <v>350363</v>
       </c>
-      <c r="G50" s="25">
+      <c r="G50" s="52">
         <v>376</v>
       </c>
       <c r="H50" s="26">
@@ -3469,10 +3511,10 @@
       <c r="I50" s="25">
         <v>325</v>
       </c>
-      <c r="J50" s="25">
+      <c r="J50" s="53">
         <v>2051</v>
       </c>
-      <c r="K50" s="25">
+      <c r="K50" s="24">
         <v>376</v>
       </c>
       <c r="L50" s="26">
@@ -3501,10 +3543,10 @@
       <c r="E51" s="24">
         <v>5428</v>
       </c>
-      <c r="F51" s="25">
+      <c r="F51" s="46">
         <v>5428</v>
       </c>
-      <c r="G51" s="25">
+      <c r="G51" s="52">
         <v>13</v>
       </c>
       <c r="H51" s="26">
@@ -3513,10 +3555,10 @@
       <c r="I51" s="25">
         <v>8</v>
       </c>
-      <c r="J51" s="25">
+      <c r="J51" s="53">
         <v>25</v>
       </c>
-      <c r="K51" s="25">
+      <c r="K51" s="24">
         <v>13</v>
       </c>
       <c r="L51" s="26">
@@ -3545,10 +3587,10 @@
       <c r="E52" s="24">
         <v>417319</v>
       </c>
-      <c r="F52" s="25">
+      <c r="F52" s="46">
         <v>806577</v>
       </c>
-      <c r="G52" s="25">
+      <c r="G52" s="52">
         <v>431</v>
       </c>
       <c r="H52" s="26">
@@ -3557,10 +3599,10 @@
       <c r="I52" s="25">
         <v>247</v>
       </c>
-      <c r="J52" s="25">
-        <v>1799</v>
-      </c>
-      <c r="K52" s="25">
+      <c r="J52" s="53">
+        <v>1798</v>
+      </c>
+      <c r="K52" s="24">
         <v>1243</v>
       </c>
       <c r="L52" s="26">
@@ -3570,7 +3612,7 @@
         <v>1428</v>
       </c>
       <c r="N52" s="25">
-        <v>8642</v>
+        <v>8640</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
@@ -3589,10 +3631,10 @@
       <c r="E53" s="24">
         <v>174639</v>
       </c>
-      <c r="F53" s="25">
+      <c r="F53" s="46">
         <v>174639</v>
       </c>
-      <c r="G53" s="25">
+      <c r="G53" s="52">
         <v>328</v>
       </c>
       <c r="H53" s="26">
@@ -3601,10 +3643,10 @@
       <c r="I53" s="25">
         <v>279</v>
       </c>
-      <c r="J53" s="25">
+      <c r="J53" s="53">
         <v>1924</v>
       </c>
-      <c r="K53" s="25">
+      <c r="K53" s="24">
         <v>328</v>
       </c>
       <c r="L53" s="26">
@@ -3633,10 +3675,10 @@
       <c r="E54" s="24">
         <v>125803</v>
       </c>
-      <c r="F54" s="25">
+      <c r="F54" s="46">
         <v>125803</v>
       </c>
-      <c r="G54" s="25">
+      <c r="G54" s="52">
         <v>141</v>
       </c>
       <c r="H54" s="26">
@@ -3645,10 +3687,10 @@
       <c r="I54" s="25">
         <v>110</v>
       </c>
-      <c r="J54" s="25">
+      <c r="J54" s="53">
         <v>612</v>
       </c>
-      <c r="K54" s="25">
+      <c r="K54" s="24">
         <v>141</v>
       </c>
       <c r="L54" s="26">
@@ -3677,10 +3719,10 @@
       <c r="E55" s="24">
         <v>110</v>
       </c>
-      <c r="F55" s="25">
+      <c r="F55" s="46">
         <v>88816</v>
       </c>
-      <c r="G55" s="25">
+      <c r="G55" s="52">
         <v>25</v>
       </c>
       <c r="H55" s="26">
@@ -3689,10 +3731,10 @@
       <c r="I55" s="25">
         <v>244</v>
       </c>
-      <c r="J55" s="25">
+      <c r="J55" s="53">
         <v>429</v>
       </c>
-      <c r="K55" s="25">
+      <c r="K55" s="24">
         <v>343</v>
       </c>
       <c r="L55" s="26">
@@ -3702,7 +3744,7 @@
         <v>1083</v>
       </c>
       <c r="N55" s="25">
-        <v>4307</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -3721,10 +3763,10 @@
       <c r="E56" s="24">
         <v>20</v>
       </c>
-      <c r="F56" s="25">
+      <c r="F56" s="46">
         <v>88706</v>
       </c>
-      <c r="G56" s="25">
+      <c r="G56" s="52">
         <v>1</v>
       </c>
       <c r="H56" s="26">
@@ -3733,10 +3775,10 @@
       <c r="I56" s="25">
         <v>15</v>
       </c>
-      <c r="J56" s="25">
+      <c r="J56" s="53">
         <v>20</v>
       </c>
-      <c r="K56" s="25">
+      <c r="K56" s="24">
         <v>318</v>
       </c>
       <c r="L56" s="26">
@@ -3746,7 +3788,7 @@
         <v>1037</v>
       </c>
       <c r="N56" s="25">
-        <v>3878</v>
+        <v>3877</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3765,10 +3807,10 @@
       <c r="E57" s="24">
         <v>8182</v>
       </c>
-      <c r="F57" s="25">
+      <c r="F57" s="46">
         <v>8182</v>
       </c>
-      <c r="G57" s="25">
+      <c r="G57" s="52">
         <v>8</v>
       </c>
       <c r="H57" s="26">
@@ -3777,10 +3819,10 @@
       <c r="I57" s="25">
         <v>9</v>
       </c>
-      <c r="J57" s="25">
+      <c r="J57" s="53">
         <v>27</v>
       </c>
-      <c r="K57" s="25">
+      <c r="K57" s="24">
         <v>8</v>
       </c>
       <c r="L57" s="26">
@@ -3809,10 +3851,10 @@
       <c r="E58" s="24">
         <v>25604</v>
       </c>
-      <c r="F58" s="25">
+      <c r="F58" s="46">
         <v>25604</v>
       </c>
-      <c r="G58" s="25">
+      <c r="G58" s="52">
         <v>91</v>
       </c>
       <c r="H58" s="26">
@@ -3821,10 +3863,10 @@
       <c r="I58" s="25">
         <v>51</v>
       </c>
-      <c r="J58" s="25">
+      <c r="J58" s="53">
         <v>465</v>
       </c>
-      <c r="K58" s="25">
+      <c r="K58" s="24">
         <v>91</v>
       </c>
       <c r="L58" s="26">
@@ -3853,10 +3895,10 @@
       <c r="E59" s="24">
         <v>32742</v>
       </c>
-      <c r="F59" s="25">
+      <c r="F59" s="46">
         <v>32742</v>
       </c>
-      <c r="G59" s="25">
+      <c r="G59" s="52">
         <v>44</v>
       </c>
       <c r="H59" s="26">
@@ -3865,10 +3907,10 @@
       <c r="I59" s="25">
         <v>45</v>
       </c>
-      <c r="J59" s="25">
+      <c r="J59" s="53">
         <v>276</v>
       </c>
-      <c r="K59" s="25">
+      <c r="K59" s="24">
         <v>44</v>
       </c>
       <c r="L59" s="26">
@@ -3897,10 +3939,10 @@
       <c r="E60" s="24">
         <v>8784</v>
       </c>
-      <c r="F60" s="25">
+      <c r="F60" s="46">
         <v>8784</v>
       </c>
-      <c r="G60" s="25">
+      <c r="G60" s="52">
         <v>13</v>
       </c>
       <c r="H60" s="26">
@@ -3909,10 +3951,10 @@
       <c r="I60" s="25">
         <v>9</v>
       </c>
-      <c r="J60" s="25">
+      <c r="J60" s="53">
         <v>58</v>
       </c>
-      <c r="K60" s="25">
+      <c r="K60" s="24">
         <v>13</v>
       </c>
       <c r="L60" s="26">
@@ -3941,10 +3983,10 @@
       <c r="E61" s="24">
         <v>13342</v>
       </c>
-      <c r="F61" s="25">
+      <c r="F61" s="46">
         <v>13374</v>
       </c>
-      <c r="G61" s="25">
+      <c r="G61" s="52">
         <v>157</v>
       </c>
       <c r="H61" s="26">
@@ -3953,10 +3995,10 @@
       <c r="I61" s="25">
         <v>635</v>
       </c>
-      <c r="J61" s="25">
-        <v>2300</v>
-      </c>
-      <c r="K61" s="25">
+      <c r="J61" s="53">
+        <v>2299</v>
+      </c>
+      <c r="K61" s="24">
         <v>161</v>
       </c>
       <c r="L61" s="26">
@@ -3966,7 +4008,7 @@
         <v>946</v>
       </c>
       <c r="N61" s="25">
-        <v>3032</v>
+        <v>3031</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -3985,10 +4027,10 @@
       <c r="E62" s="24">
         <v>32</v>
       </c>
-      <c r="F62" s="25">
+      <c r="F62" s="46">
         <v>32</v>
       </c>
-      <c r="G62" s="25">
+      <c r="G62" s="52">
         <v>4</v>
       </c>
       <c r="H62" s="26">
@@ -3997,10 +4039,10 @@
       <c r="I62" s="25">
         <v>439</v>
       </c>
-      <c r="J62" s="25">
+      <c r="J62" s="53">
         <v>732</v>
       </c>
-      <c r="K62" s="25">
+      <c r="K62" s="24">
         <v>4</v>
       </c>
       <c r="L62" s="26">
@@ -4029,10 +4071,10 @@
       <c r="E63" s="24">
         <v>183</v>
       </c>
-      <c r="F63" s="25">
+      <c r="F63" s="46">
         <v>196416</v>
       </c>
-      <c r="G63" s="25">
+      <c r="G63" s="52">
         <v>18</v>
       </c>
       <c r="H63" s="26">
@@ -4041,10 +4083,10 @@
       <c r="I63" s="25">
         <v>69</v>
       </c>
-      <c r="J63" s="25">
+      <c r="J63" s="53">
         <v>134</v>
       </c>
-      <c r="K63" s="25">
+      <c r="K63" s="24">
         <v>2972</v>
       </c>
       <c r="L63" s="26">
@@ -4054,7 +4096,7 @@
         <v>2538</v>
       </c>
       <c r="N63" s="25">
-        <v>20791</v>
+        <v>20778</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -4073,10 +4115,10 @@
       <c r="E64" s="24">
         <v>1929</v>
       </c>
-      <c r="F64" s="25">
+      <c r="F64" s="46">
         <v>1929</v>
       </c>
-      <c r="G64" s="25">
+      <c r="G64" s="52">
         <v>39</v>
       </c>
       <c r="H64" s="26">
@@ -4085,10 +4127,10 @@
       <c r="I64" s="25">
         <v>82</v>
       </c>
-      <c r="J64" s="25">
+      <c r="J64" s="53">
         <v>267</v>
       </c>
-      <c r="K64" s="25">
+      <c r="K64" s="24">
         <v>39</v>
       </c>
       <c r="L64" s="26">
@@ -4117,10 +4159,10 @@
       <c r="E65" s="24">
         <v>8</v>
       </c>
-      <c r="F65" s="25">
+      <c r="F65" s="46">
         <v>175247</v>
       </c>
-      <c r="G65" s="25">
+      <c r="G65" s="52">
         <v>1</v>
       </c>
       <c r="H65" s="26">
@@ -4129,10 +4171,10 @@
       <c r="I65" s="25">
         <v>2</v>
       </c>
-      <c r="J65" s="25">
+      <c r="J65" s="53">
         <v>2</v>
       </c>
-      <c r="K65" s="25">
+      <c r="K65" s="24">
         <v>2679</v>
       </c>
       <c r="L65" s="26">
@@ -4142,7 +4184,7 @@
         <v>2461</v>
       </c>
       <c r="N65" s="25">
-        <v>19580</v>
+        <v>19567</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -4161,10 +4203,10 @@
       <c r="E66" s="24">
         <v>83381</v>
       </c>
-      <c r="F66" s="25">
+      <c r="F66" s="46">
         <v>83381</v>
       </c>
-      <c r="G66" s="25">
+      <c r="G66" s="52">
         <v>1029</v>
       </c>
       <c r="H66" s="26">
@@ -4173,10 +4215,10 @@
       <c r="I66" s="25">
         <v>1364</v>
       </c>
-      <c r="J66" s="25">
-        <v>6314</v>
-      </c>
-      <c r="K66" s="25">
+      <c r="J66" s="53">
+        <v>6310</v>
+      </c>
+      <c r="K66" s="24">
         <v>1029</v>
       </c>
       <c r="L66" s="26">
@@ -4186,7 +4228,7 @@
         <v>1364</v>
       </c>
       <c r="N66" s="25">
-        <v>6314</v>
+        <v>6310</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -4205,10 +4247,10 @@
       <c r="E67" s="24">
         <v>6295</v>
       </c>
-      <c r="F67" s="25">
+      <c r="F67" s="46">
         <v>6295</v>
       </c>
-      <c r="G67" s="25">
+      <c r="G67" s="52">
         <v>174</v>
       </c>
       <c r="H67" s="26">
@@ -4217,10 +4259,10 @@
       <c r="I67" s="25">
         <v>614</v>
       </c>
-      <c r="J67" s="25">
-        <v>1584</v>
-      </c>
-      <c r="K67" s="25">
+      <c r="J67" s="53">
+        <v>1582</v>
+      </c>
+      <c r="K67" s="24">
         <v>174</v>
       </c>
       <c r="L67" s="26">
@@ -4230,7 +4272,7 @@
         <v>614</v>
       </c>
       <c r="N67" s="25">
-        <v>1584</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -4249,10 +4291,10 @@
       <c r="E68" s="24">
         <v>5489</v>
       </c>
-      <c r="F68" s="25">
+      <c r="F68" s="46">
         <v>5489</v>
       </c>
-      <c r="G68" s="25">
+      <c r="G68" s="52">
         <v>327</v>
       </c>
       <c r="H68" s="26">
@@ -4261,10 +4303,10 @@
       <c r="I68" s="25">
         <v>1031</v>
       </c>
-      <c r="J68" s="25">
-        <v>5543</v>
-      </c>
-      <c r="K68" s="25">
+      <c r="J68" s="53">
+        <v>5536</v>
+      </c>
+      <c r="K68" s="24">
         <v>327</v>
       </c>
       <c r="L68" s="26">
@@ -4274,7 +4316,7 @@
         <v>1031</v>
       </c>
       <c r="N68" s="25">
-        <v>5543</v>
+        <v>5536</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4293,10 +4335,10 @@
       <c r="E69" s="24">
         <v>7415</v>
       </c>
-      <c r="F69" s="25">
+      <c r="F69" s="46">
         <v>7415</v>
       </c>
-      <c r="G69" s="25">
+      <c r="G69" s="52">
         <v>317</v>
       </c>
       <c r="H69" s="26">
@@ -4305,10 +4347,10 @@
       <c r="I69" s="25">
         <v>456</v>
       </c>
-      <c r="J69" s="25">
+      <c r="J69" s="53">
         <v>1594</v>
       </c>
-      <c r="K69" s="25">
+      <c r="K69" s="24">
         <v>317</v>
       </c>
       <c r="L69" s="26">
@@ -4337,10 +4379,10 @@
       <c r="E70" s="24">
         <v>72659</v>
       </c>
-      <c r="F70" s="25">
+      <c r="F70" s="46">
         <v>72659</v>
       </c>
-      <c r="G70" s="25">
+      <c r="G70" s="52">
         <v>831</v>
       </c>
       <c r="H70" s="26">
@@ -4349,10 +4391,10 @@
       <c r="I70" s="25">
         <v>719</v>
       </c>
-      <c r="J70" s="25">
+      <c r="J70" s="53">
         <v>4543</v>
       </c>
-      <c r="K70" s="25">
+      <c r="K70" s="24">
         <v>831</v>
       </c>
       <c r="L70" s="26">
@@ -4381,10 +4423,10 @@
       <c r="E71" s="24">
         <v>5762</v>
       </c>
-      <c r="F71" s="25">
+      <c r="F71" s="46">
         <v>19057</v>
       </c>
-      <c r="G71" s="25">
+      <c r="G71" s="52">
         <v>84</v>
       </c>
       <c r="H71" s="26">
@@ -4393,10 +4435,10 @@
       <c r="I71" s="25">
         <v>110</v>
       </c>
-      <c r="J71" s="25">
+      <c r="J71" s="53">
         <v>274</v>
       </c>
-      <c r="K71" s="25">
+      <c r="K71" s="24">
         <v>236</v>
       </c>
       <c r="L71" s="26">
@@ -4425,10 +4467,10 @@
       <c r="E72" s="24">
         <v>9471</v>
       </c>
-      <c r="F72" s="25">
+      <c r="F72" s="46">
         <v>9471</v>
       </c>
-      <c r="G72" s="25">
+      <c r="G72" s="52">
         <v>111</v>
       </c>
       <c r="H72" s="26">
@@ -4437,10 +4479,10 @@
       <c r="I72" s="25">
         <v>104</v>
       </c>
-      <c r="J72" s="25">
+      <c r="J72" s="53">
         <v>347</v>
       </c>
-      <c r="K72" s="25">
+      <c r="K72" s="24">
         <v>111</v>
       </c>
       <c r="L72" s="26">
@@ -4469,10 +4511,10 @@
       <c r="E73" s="24">
         <v>3824</v>
       </c>
-      <c r="F73" s="25">
+      <c r="F73" s="46">
         <v>3824</v>
       </c>
-      <c r="G73" s="25">
+      <c r="G73" s="52">
         <v>41</v>
       </c>
       <c r="H73" s="26">
@@ -4481,10 +4523,10 @@
       <c r="I73" s="25">
         <v>79</v>
       </c>
-      <c r="J73" s="25">
+      <c r="J73" s="53">
         <v>189</v>
       </c>
-      <c r="K73" s="25">
+      <c r="K73" s="24">
         <v>41</v>
       </c>
       <c r="L73" s="26">
@@ -4513,10 +4555,10 @@
       <c r="E74" s="24">
         <v>6152</v>
       </c>
-      <c r="F74" s="25">
+      <c r="F74" s="46">
         <v>194617</v>
       </c>
-      <c r="G74" s="25">
+      <c r="G74" s="52">
         <v>455</v>
       </c>
       <c r="H74" s="26">
@@ -4525,10 +4567,10 @@
       <c r="I74" s="25">
         <v>1156</v>
       </c>
-      <c r="J74" s="25">
+      <c r="J74" s="53">
         <v>3615</v>
       </c>
-      <c r="K74" s="25">
+      <c r="K74" s="24">
         <v>969</v>
       </c>
       <c r="L74" s="26">
@@ -4538,7 +4580,7 @@
         <v>1620</v>
       </c>
       <c r="N74" s="25">
-        <v>6448</v>
+        <v>6447</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -4557,10 +4599,10 @@
       <c r="E75" s="24">
         <v>56259</v>
       </c>
-      <c r="F75" s="25">
+      <c r="F75" s="46">
         <v>58801</v>
       </c>
-      <c r="G75" s="25">
+      <c r="G75" s="52">
         <v>465</v>
       </c>
       <c r="H75" s="26">
@@ -4569,10 +4611,10 @@
       <c r="I75" s="25">
         <v>565</v>
       </c>
-      <c r="J75" s="25">
-        <v>2387</v>
-      </c>
-      <c r="K75" s="25">
+      <c r="J75" s="53">
+        <v>2386</v>
+      </c>
+      <c r="K75" s="24">
         <v>468</v>
       </c>
       <c r="L75" s="26">
@@ -4582,7 +4624,7 @@
         <v>565</v>
       </c>
       <c r="N75" s="25">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -4601,10 +4643,10 @@
       <c r="E76" s="24">
         <v>2542</v>
       </c>
-      <c r="F76" s="25">
+      <c r="F76" s="46">
         <v>2542</v>
       </c>
-      <c r="G76" s="25">
+      <c r="G76" s="52">
         <v>3</v>
       </c>
       <c r="H76" s="26">
@@ -4613,10 +4655,10 @@
       <c r="I76" s="25">
         <v>2</v>
       </c>
-      <c r="J76" s="25">
+      <c r="J76" s="53">
         <v>20</v>
       </c>
-      <c r="K76" s="25">
+      <c r="K76" s="24">
         <v>3</v>
       </c>
       <c r="L76" s="26">
@@ -4645,10 +4687,10 @@
       <c r="E77" s="24">
         <v>119</v>
       </c>
-      <c r="F77" s="25">
+      <c r="F77" s="46">
         <v>119</v>
       </c>
-      <c r="G77" s="25">
+      <c r="G77" s="52">
         <v>19</v>
       </c>
       <c r="H77" s="26">
@@ -4657,10 +4699,10 @@
       <c r="I77" s="25">
         <v>192</v>
       </c>
-      <c r="J77" s="25">
+      <c r="J77" s="53">
         <v>365</v>
       </c>
-      <c r="K77" s="25">
+      <c r="K77" s="24">
         <v>19</v>
       </c>
       <c r="L77" s="26">
@@ -4689,10 +4731,10 @@
       <c r="E78" s="24">
         <v>129570</v>
       </c>
-      <c r="F78" s="25">
+      <c r="F78" s="46">
         <v>129570</v>
       </c>
-      <c r="G78" s="25">
+      <c r="G78" s="52">
         <v>27</v>
       </c>
       <c r="H78" s="26">
@@ -4701,10 +4743,10 @@
       <c r="I78" s="25">
         <v>22</v>
       </c>
-      <c r="J78" s="25">
+      <c r="J78" s="53">
         <v>61</v>
       </c>
-      <c r="K78" s="25">
+      <c r="K78" s="24">
         <v>27</v>
       </c>
       <c r="L78" s="26">
@@ -4733,10 +4775,10 @@
       <c r="E79" s="24">
         <v>9036</v>
       </c>
-      <c r="F79" s="25">
+      <c r="F79" s="46">
         <v>453460</v>
       </c>
-      <c r="G79" s="25">
+      <c r="G79" s="52">
         <v>98</v>
       </c>
       <c r="H79" s="26">
@@ -4745,20 +4787,20 @@
       <c r="I79" s="25">
         <v>676</v>
       </c>
-      <c r="J79" s="25">
-        <v>1770</v>
-      </c>
-      <c r="K79" s="25">
-        <v>5982</v>
+      <c r="J79" s="53">
+        <v>1769</v>
+      </c>
+      <c r="K79" s="24">
+        <v>5980</v>
       </c>
       <c r="L79" s="26">
-        <v>1.3191902262603E-2</v>
+        <v>1.3187491730251801E-2</v>
       </c>
       <c r="M79" s="25">
         <v>2928</v>
       </c>
       <c r="N79" s="25">
-        <v>42633</v>
+        <v>42620</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4777,10 +4819,10 @@
       <c r="E80" s="24">
         <v>2055</v>
       </c>
-      <c r="F80" s="25">
+      <c r="F80" s="46">
         <v>2055</v>
       </c>
-      <c r="G80" s="25">
+      <c r="G80" s="52">
         <v>108</v>
       </c>
       <c r="H80" s="26">
@@ -4789,10 +4831,10 @@
       <c r="I80" s="25">
         <v>475</v>
       </c>
-      <c r="J80" s="25">
+      <c r="J80" s="53">
         <v>1258</v>
       </c>
-      <c r="K80" s="25">
+      <c r="K80" s="24">
         <v>108</v>
       </c>
       <c r="L80" s="26">
@@ -4821,10 +4863,10 @@
       <c r="E81" s="24">
         <v>27</v>
       </c>
-      <c r="F81" s="25">
+      <c r="F81" s="46">
         <v>435397</v>
       </c>
-      <c r="G81" s="25">
+      <c r="G81" s="52">
         <v>8</v>
       </c>
       <c r="H81" s="26">
@@ -4833,20 +4875,20 @@
       <c r="I81" s="25">
         <v>129</v>
       </c>
-      <c r="J81" s="25">
+      <c r="J81" s="53">
         <v>289</v>
       </c>
-      <c r="K81" s="25">
-        <v>5616</v>
+      <c r="K81" s="24">
+        <v>5614</v>
       </c>
       <c r="L81" s="26">
-        <v>1.2898573026456301E-2</v>
+        <v>1.28939795175437E-2</v>
       </c>
       <c r="M81" s="25">
         <v>2734</v>
       </c>
       <c r="N81" s="25">
-        <v>38237</v>
+        <v>38225</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -4865,10 +4907,10 @@
       <c r="E82" s="24">
         <v>381</v>
       </c>
-      <c r="F82" s="25">
+      <c r="F82" s="46">
         <v>387828</v>
       </c>
-      <c r="G82" s="25">
+      <c r="G82" s="52">
         <v>50</v>
       </c>
       <c r="H82" s="26">
@@ -4877,20 +4919,20 @@
       <c r="I82" s="25">
         <v>275</v>
       </c>
-      <c r="J82" s="25">
-        <v>800</v>
-      </c>
-      <c r="K82" s="25">
-        <v>4913</v>
+      <c r="J82" s="53">
+        <v>799</v>
+      </c>
+      <c r="K82" s="24">
+        <v>4911</v>
       </c>
       <c r="L82" s="26">
-        <v>1.26679868395268E-2</v>
+        <v>1.26628299142919E-2</v>
       </c>
       <c r="M82" s="25">
         <v>2506</v>
       </c>
       <c r="N82" s="25">
-        <v>31583</v>
+        <v>31572</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -4909,10 +4951,10 @@
       <c r="E83" s="24">
         <v>225194</v>
       </c>
-      <c r="F83" s="25">
+      <c r="F83" s="46">
         <v>379431</v>
       </c>
-      <c r="G83" s="25">
+      <c r="G83" s="52">
         <v>1803</v>
       </c>
       <c r="H83" s="26">
@@ -4921,20 +4963,20 @@
       <c r="I83" s="25">
         <v>1436</v>
       </c>
-      <c r="J83" s="25">
-        <v>10282</v>
-      </c>
-      <c r="K83" s="25">
-        <v>4541</v>
+      <c r="J83" s="53">
+        <v>10281</v>
+      </c>
+      <c r="K83" s="24">
+        <v>4539</v>
       </c>
       <c r="L83" s="26">
-        <v>1.1967920386051699E-2</v>
+        <v>1.19626493354522E-2</v>
       </c>
       <c r="M83" s="25">
         <v>2370</v>
       </c>
       <c r="N83" s="25">
-        <v>27829</v>
+        <v>27821</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -4953,10 +4995,10 @@
       <c r="E84" s="24">
         <v>12410</v>
       </c>
-      <c r="F84" s="25">
+      <c r="F84" s="46">
         <v>12410</v>
       </c>
-      <c r="G84" s="25">
+      <c r="G84" s="52">
         <v>269</v>
       </c>
       <c r="H84" s="26">
@@ -4965,10 +5007,10 @@
       <c r="I84" s="25">
         <v>548</v>
       </c>
-      <c r="J84" s="25">
+      <c r="J84" s="53">
         <v>2570</v>
       </c>
-      <c r="K84" s="25">
+      <c r="K84" s="24">
         <v>269</v>
       </c>
       <c r="L84" s="26">
@@ -4997,32 +5039,32 @@
       <c r="E85" s="24">
         <v>142043</v>
       </c>
-      <c r="F85" s="25">
+      <c r="F85" s="46">
         <v>142043</v>
       </c>
-      <c r="G85" s="25">
-        <v>2473</v>
+      <c r="G85" s="52">
+        <v>2471</v>
       </c>
       <c r="H85" s="26">
-        <v>1.7410220848616199E-2</v>
+        <v>1.7396140605309598E-2</v>
       </c>
       <c r="I85" s="25">
         <v>1620</v>
       </c>
-      <c r="J85" s="25">
-        <v>14985</v>
-      </c>
-      <c r="K85" s="25">
-        <v>2473</v>
+      <c r="J85" s="53">
+        <v>14978</v>
+      </c>
+      <c r="K85" s="24">
+        <v>2471</v>
       </c>
       <c r="L85" s="26">
-        <v>1.7410220848616199E-2</v>
+        <v>1.7396140605309598E-2</v>
       </c>
       <c r="M85" s="25">
         <v>1620</v>
       </c>
       <c r="N85" s="25">
-        <v>14985</v>
+        <v>14978</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -5041,10 +5083,10 @@
       <c r="E86" s="24">
         <v>1962</v>
       </c>
-      <c r="F86" s="25">
+      <c r="F86" s="46">
         <v>1962</v>
       </c>
-      <c r="G86" s="25">
+      <c r="G86" s="52">
         <v>133</v>
       </c>
       <c r="H86" s="26">
@@ -5053,10 +5095,10 @@
       <c r="I86" s="25">
         <v>344</v>
       </c>
-      <c r="J86" s="25">
-        <v>1614</v>
-      </c>
-      <c r="K86" s="25">
+      <c r="J86" s="53">
+        <v>1613</v>
+      </c>
+      <c r="K86" s="24">
         <v>133</v>
       </c>
       <c r="L86" s="26">
@@ -5066,7 +5108,7 @@
         <v>344</v>
       </c>
       <c r="N86" s="25">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -5085,10 +5127,10 @@
       <c r="E87" s="24">
         <v>6093</v>
       </c>
-      <c r="F87" s="25">
+      <c r="F87" s="46">
         <v>6093</v>
       </c>
-      <c r="G87" s="25">
+      <c r="G87" s="52">
         <v>191</v>
       </c>
       <c r="H87" s="26">
@@ -5097,10 +5139,10 @@
       <c r="I87" s="25">
         <v>364</v>
       </c>
-      <c r="J87" s="25">
-        <v>1353</v>
-      </c>
-      <c r="K87" s="25">
+      <c r="J87" s="53">
+        <v>1352</v>
+      </c>
+      <c r="K87" s="24">
         <v>191</v>
       </c>
       <c r="L87" s="26">
@@ -5110,7 +5152,7 @@
         <v>364</v>
       </c>
       <c r="N87" s="25">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -5129,10 +5171,10 @@
       <c r="E88" s="24">
         <v>293</v>
       </c>
-      <c r="F88" s="25">
+      <c r="F88" s="46">
         <v>310676</v>
       </c>
-      <c r="G88" s="25">
+      <c r="G88" s="52">
         <v>41</v>
       </c>
       <c r="H88" s="26">
@@ -5141,20 +5183,20 @@
       <c r="I88" s="25">
         <v>175</v>
       </c>
-      <c r="J88" s="25">
+      <c r="J88" s="53">
         <v>318</v>
       </c>
-      <c r="K88" s="25">
-        <v>4696</v>
+      <c r="K88" s="24">
+        <v>4694</v>
       </c>
       <c r="L88" s="26">
-        <v>1.5115425716823901E-2</v>
+        <v>1.5108988141987099E-2</v>
       </c>
       <c r="M88" s="25">
         <v>2667</v>
       </c>
       <c r="N88" s="25">
-        <v>31971</v>
+        <v>31960</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -5173,10 +5215,10 @@
       <c r="E89" s="24">
         <v>149110</v>
       </c>
-      <c r="F89" s="25">
+      <c r="F89" s="46">
         <v>154731</v>
       </c>
-      <c r="G89" s="25">
+      <c r="G89" s="52">
         <v>1591</v>
       </c>
       <c r="H89" s="26">
@@ -5185,10 +5227,10 @@
       <c r="I89" s="25">
         <v>1723</v>
       </c>
-      <c r="J89" s="25">
-        <v>11307</v>
-      </c>
-      <c r="K89" s="25">
+      <c r="J89" s="53">
+        <v>11305</v>
+      </c>
+      <c r="K89" s="24">
         <v>1697</v>
       </c>
       <c r="L89" s="26">
@@ -5198,7 +5240,7 @@
         <v>1771</v>
       </c>
       <c r="N89" s="25">
-        <v>12034</v>
+        <v>12032</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -5217,10 +5259,10 @@
       <c r="E90" s="24">
         <v>5621</v>
       </c>
-      <c r="F90" s="25">
+      <c r="F90" s="46">
         <v>5621</v>
       </c>
-      <c r="G90" s="25">
+      <c r="G90" s="52">
         <v>106</v>
       </c>
       <c r="H90" s="26">
@@ -5229,10 +5271,10 @@
       <c r="I90" s="25">
         <v>156</v>
       </c>
-      <c r="J90" s="25">
+      <c r="J90" s="53">
         <v>727</v>
       </c>
-      <c r="K90" s="25">
+      <c r="K90" s="24">
         <v>106</v>
       </c>
       <c r="L90" s="26">
@@ -5261,10 +5303,10 @@
       <c r="E91" s="24">
         <v>7326</v>
       </c>
-      <c r="F91" s="25">
+      <c r="F91" s="46">
         <v>7326</v>
       </c>
-      <c r="G91" s="25">
+      <c r="G91" s="52">
         <v>201</v>
       </c>
       <c r="H91" s="26">
@@ -5273,10 +5315,10 @@
       <c r="I91" s="25">
         <v>314</v>
       </c>
-      <c r="J91" s="25">
-        <v>1542</v>
-      </c>
-      <c r="K91" s="25">
+      <c r="J91" s="53">
+        <v>1541</v>
+      </c>
+      <c r="K91" s="24">
         <v>201</v>
       </c>
       <c r="L91" s="26">
@@ -5286,7 +5328,7 @@
         <v>314</v>
       </c>
       <c r="N91" s="25">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -5305,10 +5347,10 @@
       <c r="E92" s="24">
         <v>71220</v>
       </c>
-      <c r="F92" s="25">
+      <c r="F92" s="46">
         <v>141847</v>
       </c>
-      <c r="G92" s="25">
+      <c r="G92" s="52">
         <v>1341</v>
       </c>
       <c r="H92" s="26">
@@ -5317,20 +5359,20 @@
       <c r="I92" s="25">
         <v>1608</v>
       </c>
-      <c r="J92" s="25">
-        <v>10327</v>
-      </c>
-      <c r="K92" s="25">
-        <v>2788</v>
+      <c r="J92" s="53">
+        <v>10325</v>
+      </c>
+      <c r="K92" s="24">
+        <v>2786</v>
       </c>
       <c r="L92" s="26">
-        <v>1.9654980366169101E-2</v>
+        <v>1.9640880667197699E-2</v>
       </c>
       <c r="M92" s="25">
         <v>2021</v>
       </c>
       <c r="N92" s="25">
-        <v>19327</v>
+        <v>19320</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -5349,10 +5391,10 @@
       <c r="E93" s="24">
         <v>3201</v>
       </c>
-      <c r="F93" s="25">
+      <c r="F93" s="46">
         <v>3201</v>
       </c>
-      <c r="G93" s="25">
+      <c r="G93" s="52">
         <v>112</v>
       </c>
       <c r="H93" s="26">
@@ -5361,10 +5403,10 @@
       <c r="I93" s="25">
         <v>195</v>
       </c>
-      <c r="J93" s="25">
+      <c r="J93" s="53">
         <v>854</v>
       </c>
-      <c r="K93" s="25">
+      <c r="K93" s="24">
         <v>112</v>
       </c>
       <c r="L93" s="26">
@@ -5393,32 +5435,32 @@
       <c r="E94" s="24">
         <v>29929</v>
       </c>
-      <c r="F94" s="25">
+      <c r="F94" s="46">
         <v>29929</v>
       </c>
-      <c r="G94" s="25">
-        <v>650</v>
+      <c r="G94" s="52">
+        <v>649</v>
       </c>
       <c r="H94" s="26">
-        <v>2.1718066089745702E-2</v>
+        <v>2.1684653680376802E-2</v>
       </c>
       <c r="I94" s="25">
         <v>676</v>
       </c>
-      <c r="J94" s="25">
-        <v>3698</v>
-      </c>
-      <c r="K94" s="25">
-        <v>650</v>
+      <c r="J94" s="53">
+        <v>3695</v>
+      </c>
+      <c r="K94" s="24">
+        <v>649</v>
       </c>
       <c r="L94" s="26">
-        <v>2.1718066089745702E-2</v>
+        <v>2.1684653680376802E-2</v>
       </c>
       <c r="M94" s="25">
         <v>676</v>
       </c>
       <c r="N94" s="25">
-        <v>3698</v>
+        <v>3695</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -5437,10 +5479,10 @@
       <c r="E95" s="24">
         <v>3019</v>
       </c>
-      <c r="F95" s="25">
+      <c r="F95" s="46">
         <v>3019</v>
       </c>
-      <c r="G95" s="25">
+      <c r="G95" s="52">
         <v>47</v>
       </c>
       <c r="H95" s="26">
@@ -5449,10 +5491,10 @@
       <c r="I95" s="25">
         <v>77</v>
       </c>
-      <c r="J95" s="25">
+      <c r="J95" s="53">
         <v>373</v>
       </c>
-      <c r="K95" s="25">
+      <c r="K95" s="24">
         <v>47</v>
       </c>
       <c r="L95" s="26">
@@ -5481,32 +5523,32 @@
       <c r="E96" s="24">
         <v>29930</v>
       </c>
-      <c r="F96" s="25">
+      <c r="F96" s="46">
         <v>29930</v>
       </c>
-      <c r="G96" s="25">
-        <v>434</v>
+      <c r="G96" s="52">
+        <v>433</v>
       </c>
       <c r="H96" s="26">
-        <v>1.45005011693952E-2</v>
+        <v>1.44670898763782E-2</v>
       </c>
       <c r="I96" s="25">
         <v>505</v>
       </c>
-      <c r="J96" s="25">
-        <v>3061</v>
-      </c>
-      <c r="K96" s="25">
-        <v>434</v>
+      <c r="J96" s="53">
+        <v>3059</v>
+      </c>
+      <c r="K96" s="24">
+        <v>433</v>
       </c>
       <c r="L96" s="26">
-        <v>1.45005011693952E-2</v>
+        <v>1.44670898763782E-2</v>
       </c>
       <c r="M96" s="25">
         <v>505</v>
       </c>
       <c r="N96" s="25">
-        <v>3061</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -5525,10 +5567,10 @@
       <c r="E97" s="24">
         <v>5270</v>
       </c>
-      <c r="F97" s="25">
+      <c r="F97" s="46">
         <v>5270</v>
       </c>
-      <c r="G97" s="25">
+      <c r="G97" s="52">
         <v>283</v>
       </c>
       <c r="H97" s="26">
@@ -5537,10 +5579,10 @@
       <c r="I97" s="25">
         <v>334</v>
       </c>
-      <c r="J97" s="25">
+      <c r="J97" s="53">
         <v>1462</v>
       </c>
-      <c r="K97" s="25">
+      <c r="K97" s="24">
         <v>283</v>
       </c>
       <c r="L97" s="26">
@@ -5569,10 +5611,10 @@
       <c r="E98" s="24">
         <v>16511</v>
       </c>
-      <c r="F98" s="25">
+      <c r="F98" s="46">
         <v>16511</v>
       </c>
-      <c r="G98" s="25">
+      <c r="G98" s="52">
         <v>232</v>
       </c>
       <c r="H98" s="26">
@@ -5581,10 +5623,10 @@
       <c r="I98" s="25">
         <v>442</v>
       </c>
-      <c r="J98" s="25">
+      <c r="J98" s="53">
         <v>1346</v>
       </c>
-      <c r="K98" s="25">
+      <c r="K98" s="24">
         <v>232</v>
       </c>
       <c r="L98" s="26">
@@ -5613,10 +5655,10 @@
       <c r="E99" s="24">
         <v>6236</v>
       </c>
-      <c r="F99" s="25">
+      <c r="F99" s="46">
         <v>6236</v>
       </c>
-      <c r="G99" s="25">
+      <c r="G99" s="52">
         <v>228</v>
       </c>
       <c r="H99" s="26">
@@ -5625,10 +5667,10 @@
       <c r="I99" s="25">
         <v>324</v>
       </c>
-      <c r="J99" s="25">
-        <v>1552</v>
-      </c>
-      <c r="K99" s="25">
+      <c r="J99" s="53">
+        <v>1550</v>
+      </c>
+      <c r="K99" s="24">
         <v>228</v>
       </c>
       <c r="L99" s="26">
@@ -5638,7 +5680,7 @@
         <v>324</v>
       </c>
       <c r="N99" s="25">
-        <v>1552</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -5657,10 +5699,10 @@
       <c r="E100" s="24">
         <v>7041</v>
       </c>
-      <c r="F100" s="25">
+      <c r="F100" s="46">
         <v>7041</v>
       </c>
-      <c r="G100" s="25">
+      <c r="G100" s="52">
         <v>174</v>
       </c>
       <c r="H100" s="26">
@@ -5669,10 +5711,10 @@
       <c r="I100" s="25">
         <v>286</v>
       </c>
-      <c r="J100" s="25">
+      <c r="J100" s="53">
         <v>1462</v>
       </c>
-      <c r="K100" s="25">
+      <c r="K100" s="24">
         <v>174</v>
       </c>
       <c r="L100" s="26">
@@ -5701,10 +5743,10 @@
       <c r="E101" s="24">
         <v>758</v>
       </c>
-      <c r="F101" s="25">
+      <c r="F101" s="46">
         <v>507653</v>
       </c>
-      <c r="G101" s="25">
+      <c r="G101" s="52">
         <v>160</v>
       </c>
       <c r="H101" s="26">
@@ -5713,20 +5755,20 @@
       <c r="I101" s="25">
         <v>1470</v>
       </c>
-      <c r="J101" s="25">
+      <c r="J101" s="53">
         <v>2997</v>
       </c>
-      <c r="K101" s="25">
-        <v>10957</v>
+      <c r="K101" s="24">
+        <v>10955</v>
       </c>
       <c r="L101" s="26">
-        <v>2.15836407940069E-2</v>
+        <v>2.1579701095039299E-2</v>
       </c>
       <c r="M101" s="25">
         <v>4390</v>
       </c>
       <c r="N101" s="25">
-        <v>169501</v>
+        <v>169467</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -5745,10 +5787,10 @@
       <c r="E102" s="24">
         <v>678</v>
       </c>
-      <c r="F102" s="25">
+      <c r="F102" s="46">
         <v>85696</v>
       </c>
-      <c r="G102" s="25">
+      <c r="G102" s="52">
         <v>133</v>
       </c>
       <c r="H102" s="26">
@@ -5757,10 +5799,10 @@
       <c r="I102" s="25">
         <v>1405</v>
       </c>
-      <c r="J102" s="25">
-        <v>3734</v>
-      </c>
-      <c r="K102" s="25">
+      <c r="J102" s="53">
+        <v>3732</v>
+      </c>
+      <c r="K102" s="24">
         <v>404</v>
       </c>
       <c r="L102" s="26">
@@ -5770,7 +5812,7 @@
         <v>1877</v>
       </c>
       <c r="N102" s="25">
-        <v>5762</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -5789,10 +5831,10 @@
       <c r="E103" s="24">
         <v>85018</v>
       </c>
-      <c r="F103" s="25">
+      <c r="F103" s="46">
         <v>85018</v>
       </c>
-      <c r="G103" s="25">
+      <c r="G103" s="52">
         <v>271</v>
       </c>
       <c r="H103" s="26">
@@ -5801,10 +5843,10 @@
       <c r="I103" s="25">
         <v>858</v>
       </c>
-      <c r="J103" s="25">
-        <v>2028</v>
-      </c>
-      <c r="K103" s="25">
+      <c r="J103" s="53">
+        <v>2027</v>
+      </c>
+      <c r="K103" s="24">
         <v>271</v>
       </c>
       <c r="L103" s="26">
@@ -5814,7 +5856,7 @@
         <v>858</v>
       </c>
       <c r="N103" s="25">
-        <v>2028</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -5833,10 +5875,10 @@
       <c r="E104" s="24">
         <v>286524</v>
       </c>
-      <c r="F104" s="25">
+      <c r="F104" s="46">
         <v>308234</v>
       </c>
-      <c r="G104" s="25">
+      <c r="G104" s="52">
         <v>2645</v>
       </c>
       <c r="H104" s="26">
@@ -5845,10 +5887,10 @@
       <c r="I104" s="25">
         <v>3470</v>
       </c>
-      <c r="J104" s="25">
-        <v>15677</v>
-      </c>
-      <c r="K104" s="25">
+      <c r="J104" s="53">
+        <v>15675</v>
+      </c>
+      <c r="K104" s="24">
         <v>3143</v>
       </c>
       <c r="L104" s="26">
@@ -5858,7 +5900,7 @@
         <v>3577</v>
       </c>
       <c r="N104" s="25">
-        <v>18437</v>
+        <v>18435</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -5877,10 +5919,10 @@
       <c r="E105" s="24">
         <v>8685</v>
       </c>
-      <c r="F105" s="25">
+      <c r="F105" s="46">
         <v>8685</v>
       </c>
-      <c r="G105" s="25">
+      <c r="G105" s="52">
         <v>199</v>
       </c>
       <c r="H105" s="26">
@@ -5889,10 +5931,10 @@
       <c r="I105" s="25">
         <v>412</v>
       </c>
-      <c r="J105" s="25">
+      <c r="J105" s="53">
         <v>874</v>
       </c>
-      <c r="K105" s="25">
+      <c r="K105" s="24">
         <v>199</v>
       </c>
       <c r="L105" s="26">
@@ -5921,10 +5963,10 @@
       <c r="E106" s="24">
         <v>13025</v>
       </c>
-      <c r="F106" s="25">
+      <c r="F106" s="46">
         <v>13025</v>
       </c>
-      <c r="G106" s="25">
+      <c r="G106" s="52">
         <v>299</v>
       </c>
       <c r="H106" s="26">
@@ -5933,10 +5975,10 @@
       <c r="I106" s="25">
         <v>649</v>
       </c>
-      <c r="J106" s="25">
+      <c r="J106" s="53">
         <v>1886</v>
       </c>
-      <c r="K106" s="25">
+      <c r="K106" s="24">
         <v>299</v>
       </c>
       <c r="L106" s="26">
@@ -5965,10 +6007,10 @@
       <c r="E107" s="24">
         <v>3541</v>
       </c>
-      <c r="F107" s="25">
+      <c r="F107" s="46">
         <v>67556</v>
       </c>
-      <c r="G107" s="25">
+      <c r="G107" s="52">
         <v>389</v>
       </c>
       <c r="H107" s="26">
@@ -5977,20 +6019,20 @@
       <c r="I107" s="25">
         <v>2839</v>
       </c>
-      <c r="J107" s="25">
-        <v>9349</v>
-      </c>
-      <c r="K107" s="25">
-        <v>4862</v>
+      <c r="J107" s="53">
+        <v>9348</v>
+      </c>
+      <c r="K107" s="24">
+        <v>4860</v>
       </c>
       <c r="L107" s="26">
-        <v>7.1969921250518001E-2</v>
+        <v>7.1940316182130301E-2</v>
       </c>
       <c r="M107" s="25">
         <v>4387</v>
       </c>
       <c r="N107" s="25">
-        <v>108583</v>
+        <v>108561</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -6009,10 +6051,10 @@
       <c r="E108" s="24">
         <v>3742</v>
       </c>
-      <c r="F108" s="25">
+      <c r="F108" s="46">
         <v>3742</v>
       </c>
-      <c r="G108" s="25">
+      <c r="G108" s="52">
         <v>431</v>
       </c>
       <c r="H108" s="26">
@@ -6021,10 +6063,10 @@
       <c r="I108" s="25">
         <v>2621</v>
       </c>
-      <c r="J108" s="25">
-        <v>10172</v>
-      </c>
-      <c r="K108" s="25">
+      <c r="J108" s="53">
+        <v>10169</v>
+      </c>
+      <c r="K108" s="24">
         <v>431</v>
       </c>
       <c r="L108" s="26">
@@ -6034,7 +6076,7 @@
         <v>2621</v>
       </c>
       <c r="N108" s="25">
-        <v>10172</v>
+        <v>10169</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -6053,10 +6095,10 @@
       <c r="E109" s="24">
         <v>4249</v>
       </c>
-      <c r="F109" s="25">
+      <c r="F109" s="46">
         <v>4249</v>
       </c>
-      <c r="G109" s="25">
+      <c r="G109" s="52">
         <v>1037</v>
       </c>
       <c r="H109" s="26">
@@ -6065,10 +6107,10 @@
       <c r="I109" s="25">
         <v>4122</v>
       </c>
-      <c r="J109" s="25">
-        <v>31486</v>
-      </c>
-      <c r="K109" s="25">
+      <c r="J109" s="53">
+        <v>31485</v>
+      </c>
+      <c r="K109" s="24">
         <v>1037</v>
       </c>
       <c r="L109" s="26">
@@ -6078,7 +6120,7 @@
         <v>4122</v>
       </c>
       <c r="N109" s="25">
-        <v>31486</v>
+        <v>31485</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -6097,32 +6139,32 @@
       <c r="E110" s="24">
         <v>9106</v>
       </c>
-      <c r="F110" s="25">
+      <c r="F110" s="46">
         <v>9106</v>
       </c>
-      <c r="G110" s="25">
-        <v>905</v>
+      <c r="G110" s="52">
+        <v>904</v>
       </c>
       <c r="H110" s="26">
-        <v>9.9385020865363494E-2</v>
+        <v>9.9275203162749806E-2</v>
       </c>
       <c r="I110" s="25">
         <v>3441</v>
       </c>
-      <c r="J110" s="25">
-        <v>20003</v>
-      </c>
-      <c r="K110" s="25">
-        <v>905</v>
+      <c r="J110" s="53">
+        <v>19995</v>
+      </c>
+      <c r="K110" s="24">
+        <v>904</v>
       </c>
       <c r="L110" s="26">
-        <v>9.9385020865363494E-2</v>
+        <v>9.9275203162749806E-2</v>
       </c>
       <c r="M110" s="25">
         <v>3441</v>
       </c>
       <c r="N110" s="25">
-        <v>20003</v>
+        <v>19995</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -6141,10 +6183,10 @@
       <c r="E111" s="24">
         <v>4419</v>
       </c>
-      <c r="F111" s="25">
+      <c r="F111" s="46">
         <v>42799</v>
       </c>
-      <c r="G111" s="25">
+      <c r="G111" s="52">
         <v>526</v>
       </c>
       <c r="H111" s="26">
@@ -6153,20 +6195,20 @@
       <c r="I111" s="25">
         <v>2290</v>
       </c>
-      <c r="J111" s="25">
-        <v>7577</v>
-      </c>
-      <c r="K111" s="25">
-        <v>1319</v>
+      <c r="J111" s="53">
+        <v>7576</v>
+      </c>
+      <c r="K111" s="24">
+        <v>1318</v>
       </c>
       <c r="L111" s="26">
-        <v>3.0818477067221101E-2</v>
+        <v>3.07951120353279E-2</v>
       </c>
       <c r="M111" s="25">
         <v>2992</v>
       </c>
       <c r="N111" s="25">
-        <v>13388</v>
+        <v>13386</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
@@ -6185,32 +6227,32 @@
       <c r="E112" s="24">
         <v>24452</v>
       </c>
-      <c r="F112" s="25">
+      <c r="F112" s="46">
         <v>24452</v>
       </c>
-      <c r="G112" s="25">
-        <v>251</v>
+      <c r="G112" s="52">
+        <v>250</v>
       </c>
       <c r="H112" s="26">
-        <v>1.0265008997218999E-2</v>
+        <v>1.02241125470309E-2</v>
       </c>
       <c r="I112" s="25">
         <v>470</v>
       </c>
-      <c r="J112" s="25">
-        <v>1152</v>
-      </c>
-      <c r="K112" s="25">
-        <v>251</v>
+      <c r="J112" s="53">
+        <v>1151</v>
+      </c>
+      <c r="K112" s="24">
+        <v>250</v>
       </c>
       <c r="L112" s="26">
-        <v>1.0265008997218999E-2</v>
+        <v>1.02241125470309E-2</v>
       </c>
       <c r="M112" s="25">
         <v>470</v>
       </c>
       <c r="N112" s="25">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -6229,10 +6271,10 @@
       <c r="E113" s="24">
         <v>8823</v>
       </c>
-      <c r="F113" s="25">
+      <c r="F113" s="46">
         <v>8823</v>
       </c>
-      <c r="G113" s="25">
+      <c r="G113" s="52">
         <v>138</v>
       </c>
       <c r="H113" s="26">
@@ -6241,10 +6283,10 @@
       <c r="I113" s="25">
         <v>225</v>
       </c>
-      <c r="J113" s="25">
+      <c r="J113" s="53">
         <v>602</v>
       </c>
-      <c r="K113" s="25">
+      <c r="K113" s="24">
         <v>138</v>
       </c>
       <c r="L113" s="26">
@@ -6273,10 +6315,10 @@
       <c r="E114" s="24">
         <v>4542</v>
       </c>
-      <c r="F114" s="25">
+      <c r="F114" s="46">
         <v>4542</v>
       </c>
-      <c r="G114" s="25">
+      <c r="G114" s="52">
         <v>318</v>
       </c>
       <c r="H114" s="26">
@@ -6285,10 +6327,10 @@
       <c r="I114" s="25">
         <v>880</v>
       </c>
-      <c r="J114" s="25">
+      <c r="J114" s="53">
         <v>3007</v>
       </c>
-      <c r="K114" s="25">
+      <c r="K114" s="24">
         <v>318</v>
       </c>
       <c r="L114" s="26">
@@ -6317,10 +6359,10 @@
       <c r="E115" s="24">
         <v>12</v>
       </c>
-      <c r="F115" s="25">
+      <c r="F115" s="46">
         <v>563</v>
       </c>
-      <c r="G115" s="25">
+      <c r="G115" s="52">
         <v>7</v>
       </c>
       <c r="H115" s="26">
@@ -6329,10 +6371,10 @@
       <c r="I115" s="25">
         <v>41</v>
       </c>
-      <c r="J115" s="25">
+      <c r="J115" s="53">
         <v>61</v>
       </c>
-      <c r="K115" s="25">
+      <c r="K115" s="24">
         <v>86</v>
       </c>
       <c r="L115" s="26">
@@ -6361,10 +6403,10 @@
       <c r="E116" s="24">
         <v>365</v>
       </c>
-      <c r="F116" s="25">
+      <c r="F116" s="46">
         <v>365</v>
       </c>
-      <c r="G116" s="25">
+      <c r="G116" s="52">
         <v>40</v>
       </c>
       <c r="H116" s="26">
@@ -6373,10 +6415,10 @@
       <c r="I116" s="25">
         <v>219</v>
       </c>
-      <c r="J116" s="25">
+      <c r="J116" s="53">
         <v>624</v>
       </c>
-      <c r="K116" s="25">
+      <c r="K116" s="24">
         <v>40</v>
       </c>
       <c r="L116" s="26">
@@ -6405,10 +6447,10 @@
       <c r="E117" s="24">
         <v>184</v>
       </c>
-      <c r="F117" s="25">
+      <c r="F117" s="46">
         <v>184</v>
       </c>
-      <c r="G117" s="25">
+      <c r="G117" s="52">
         <v>39</v>
       </c>
       <c r="H117" s="26">
@@ -6417,10 +6459,10 @@
       <c r="I117" s="25">
         <v>135</v>
       </c>
-      <c r="J117" s="25">
+      <c r="J117" s="53">
         <v>365</v>
       </c>
-      <c r="K117" s="25">
+      <c r="K117" s="24">
         <v>39</v>
       </c>
       <c r="L117" s="26">
@@ -6449,10 +6491,10 @@
       <c r="E118" s="24">
         <v>2</v>
       </c>
-      <c r="F118" s="25">
+      <c r="F118" s="46">
         <v>2</v>
       </c>
-      <c r="G118" s="25">
+      <c r="G118" s="52">
         <v>0</v>
       </c>
       <c r="H118" s="26">
@@ -6461,10 +6503,10 @@
       <c r="I118" s="25">
         <v>0</v>
       </c>
-      <c r="J118" s="25">
+      <c r="J118" s="53">
         <v>0</v>
       </c>
-      <c r="K118" s="25">
+      <c r="K118" s="24">
         <v>0</v>
       </c>
       <c r="L118" s="26">
@@ -6493,10 +6535,10 @@
       <c r="E119" s="24">
         <v>3549</v>
       </c>
-      <c r="F119" s="25">
+      <c r="F119" s="46">
         <v>4119</v>
       </c>
-      <c r="G119" s="25">
+      <c r="G119" s="52">
         <v>721</v>
       </c>
       <c r="H119" s="26">
@@ -6505,10 +6547,10 @@
       <c r="I119" s="25">
         <v>3979</v>
       </c>
-      <c r="J119" s="25">
-        <v>23668</v>
-      </c>
-      <c r="K119" s="25">
+      <c r="J119" s="53">
+        <v>23661</v>
+      </c>
+      <c r="K119" s="24">
         <v>781</v>
       </c>
       <c r="L119" s="26">
@@ -6518,7 +6560,7 @@
         <v>3990</v>
       </c>
       <c r="N119" s="25">
-        <v>24185</v>
+        <v>24178</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
@@ -6537,10 +6579,10 @@
       <c r="E120" s="24">
         <v>570</v>
       </c>
-      <c r="F120" s="25">
+      <c r="F120" s="46">
         <v>570</v>
       </c>
-      <c r="G120" s="25">
+      <c r="G120" s="52">
         <v>60</v>
       </c>
       <c r="H120" s="26">
@@ -6549,10 +6591,10 @@
       <c r="I120" s="25">
         <v>257</v>
       </c>
-      <c r="J120" s="25">
+      <c r="J120" s="53">
         <v>517</v>
       </c>
-      <c r="K120" s="25">
+      <c r="K120" s="24">
         <v>60</v>
       </c>
       <c r="L120" s="26">
@@ -6581,10 +6623,10 @@
       <c r="E121" s="24">
         <v>529</v>
       </c>
-      <c r="F121" s="25">
+      <c r="F121" s="46">
         <v>1636</v>
       </c>
-      <c r="G121" s="25">
+      <c r="G121" s="52">
         <v>114</v>
       </c>
       <c r="H121" s="26">
@@ -6593,10 +6635,10 @@
       <c r="I121" s="25">
         <v>321</v>
       </c>
-      <c r="J121" s="25">
+      <c r="J121" s="53">
         <v>565</v>
       </c>
-      <c r="K121" s="25">
+      <c r="K121" s="24">
         <v>305</v>
       </c>
       <c r="L121" s="26">
@@ -6625,10 +6667,10 @@
       <c r="E122" s="24">
         <v>1107</v>
       </c>
-      <c r="F122" s="25">
+      <c r="F122" s="46">
         <v>1107</v>
       </c>
-      <c r="G122" s="25">
+      <c r="G122" s="52">
         <v>191</v>
       </c>
       <c r="H122" s="26">
@@ -6637,10 +6679,10 @@
       <c r="I122" s="25">
         <v>484</v>
       </c>
-      <c r="J122" s="25">
+      <c r="J122" s="53">
         <v>938</v>
       </c>
-      <c r="K122" s="25">
+      <c r="K122" s="24">
         <v>191</v>
       </c>
       <c r="L122" s="26">
@@ -6669,10 +6711,10 @@
       <c r="E123" s="24">
         <v>346</v>
       </c>
-      <c r="F123" s="25">
+      <c r="F123" s="46">
         <v>2695</v>
       </c>
-      <c r="G123" s="25">
+      <c r="G123" s="52">
         <v>62</v>
       </c>
       <c r="H123" s="26">
@@ -6681,10 +6723,10 @@
       <c r="I123" s="25">
         <v>225</v>
       </c>
-      <c r="J123" s="25">
+      <c r="J123" s="53">
         <v>421</v>
       </c>
-      <c r="K123" s="25">
+      <c r="K123" s="24">
         <v>291</v>
       </c>
       <c r="L123" s="26">
@@ -6713,10 +6755,10 @@
       <c r="E124" s="24">
         <v>2259</v>
       </c>
-      <c r="F124" s="25">
+      <c r="F124" s="46">
         <v>2259</v>
       </c>
-      <c r="G124" s="25">
+      <c r="G124" s="52">
         <v>211</v>
       </c>
       <c r="H124" s="26">
@@ -6725,10 +6767,10 @@
       <c r="I124" s="25">
         <v>727</v>
       </c>
-      <c r="J124" s="25">
+      <c r="J124" s="53">
         <v>1779</v>
       </c>
-      <c r="K124" s="25">
+      <c r="K124" s="24">
         <v>211</v>
       </c>
       <c r="L124" s="26">
@@ -6757,10 +6799,10 @@
       <c r="E125" s="24">
         <v>45</v>
       </c>
-      <c r="F125" s="25">
+      <c r="F125" s="46">
         <v>45</v>
       </c>
-      <c r="G125" s="25">
+      <c r="G125" s="52">
         <v>13</v>
       </c>
       <c r="H125" s="26">
@@ -6769,10 +6811,10 @@
       <c r="I125" s="25">
         <v>24</v>
       </c>
-      <c r="J125" s="25">
+      <c r="J125" s="53">
         <v>36</v>
       </c>
-      <c r="K125" s="25">
+      <c r="K125" s="24">
         <v>13</v>
       </c>
       <c r="L125" s="26">
@@ -6801,10 +6843,10 @@
       <c r="E126" s="24">
         <v>45</v>
       </c>
-      <c r="F126" s="25">
+      <c r="F126" s="46">
         <v>45</v>
       </c>
-      <c r="G126" s="25">
+      <c r="G126" s="52">
         <v>5</v>
       </c>
       <c r="H126" s="26">
@@ -6813,10 +6855,10 @@
       <c r="I126" s="25">
         <v>11</v>
       </c>
-      <c r="J126" s="25">
+      <c r="J126" s="53">
         <v>19</v>
       </c>
-      <c r="K126" s="25">
+      <c r="K126" s="24">
         <v>5</v>
       </c>
       <c r="L126" s="26">
@@ -6845,10 +6887,10 @@
       <c r="E127" s="24">
         <v>53</v>
       </c>
-      <c r="F127" s="25">
+      <c r="F127" s="46">
         <v>9064</v>
       </c>
-      <c r="G127" s="25">
+      <c r="G127" s="52">
         <v>22</v>
       </c>
       <c r="H127" s="26">
@@ -6857,10 +6899,10 @@
       <c r="I127" s="25">
         <v>479</v>
       </c>
-      <c r="J127" s="25">
+      <c r="J127" s="53">
         <v>1046</v>
       </c>
-      <c r="K127" s="25">
+      <c r="K127" s="24">
         <v>663</v>
       </c>
       <c r="L127" s="26">
@@ -6870,7 +6912,7 @@
         <v>2830</v>
       </c>
       <c r="N127" s="25">
-        <v>18499</v>
+        <v>18494</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
@@ -6889,10 +6931,10 @@
       <c r="E128" s="24">
         <v>5704</v>
       </c>
-      <c r="F128" s="25">
+      <c r="F128" s="46">
         <v>5704</v>
       </c>
-      <c r="G128" s="25">
+      <c r="G128" s="52">
         <v>261</v>
       </c>
       <c r="H128" s="26">
@@ -6901,10 +6943,10 @@
       <c r="I128" s="25">
         <v>623</v>
       </c>
-      <c r="J128" s="25">
+      <c r="J128" s="53">
         <v>1856</v>
       </c>
-      <c r="K128" s="25">
+      <c r="K128" s="24">
         <v>261</v>
       </c>
       <c r="L128" s="26">
@@ -6933,10 +6975,10 @@
       <c r="E129" s="24">
         <v>2556</v>
       </c>
-      <c r="F129" s="25">
+      <c r="F129" s="46">
         <v>2556</v>
       </c>
-      <c r="G129" s="25">
+      <c r="G129" s="52">
         <v>244</v>
       </c>
       <c r="H129" s="26">
@@ -6945,10 +6987,10 @@
       <c r="I129" s="25">
         <v>1644</v>
       </c>
-      <c r="J129" s="25">
+      <c r="J129" s="53">
         <v>6319</v>
       </c>
-      <c r="K129" s="25">
+      <c r="K129" s="24">
         <v>244</v>
       </c>
       <c r="L129" s="26">
@@ -6977,10 +7019,10 @@
       <c r="E130" s="24">
         <v>372</v>
       </c>
-      <c r="F130" s="25">
+      <c r="F130" s="46">
         <v>372</v>
       </c>
-      <c r="G130" s="25">
+      <c r="G130" s="52">
         <v>56</v>
       </c>
       <c r="H130" s="26">
@@ -6989,10 +7031,10 @@
       <c r="I130" s="25">
         <v>233</v>
       </c>
-      <c r="J130" s="25">
+      <c r="J130" s="53">
         <v>816</v>
       </c>
-      <c r="K130" s="25">
+      <c r="K130" s="24">
         <v>56</v>
       </c>
       <c r="L130" s="26">
@@ -7021,10 +7063,10 @@
       <c r="E131" s="24">
         <v>120</v>
       </c>
-      <c r="F131" s="25">
+      <c r="F131" s="46">
         <v>120</v>
       </c>
-      <c r="G131" s="25">
+      <c r="G131" s="52">
         <v>43</v>
       </c>
       <c r="H131" s="26">
@@ -7033,10 +7075,10 @@
       <c r="I131" s="25">
         <v>628</v>
       </c>
-      <c r="J131" s="25">
+      <c r="J131" s="53">
         <v>2157</v>
       </c>
-      <c r="K131" s="25">
+      <c r="K131" s="24">
         <v>43</v>
       </c>
       <c r="L131" s="26">
@@ -7065,10 +7107,10 @@
       <c r="E132" s="24">
         <v>259</v>
       </c>
-      <c r="F132" s="25">
+      <c r="F132" s="46">
         <v>259</v>
       </c>
-      <c r="G132" s="25">
+      <c r="G132" s="52">
         <v>37</v>
       </c>
       <c r="H132" s="26">
@@ -7077,10 +7119,10 @@
       <c r="I132" s="25">
         <v>1520</v>
       </c>
-      <c r="J132" s="25">
-        <v>6305</v>
-      </c>
-      <c r="K132" s="25">
+      <c r="J132" s="53">
+        <v>6300</v>
+      </c>
+      <c r="K132" s="24">
         <v>37</v>
       </c>
       <c r="L132" s="26">
@@ -7090,7 +7132,7 @@
         <v>1520</v>
       </c>
       <c r="N132" s="25">
-        <v>6305</v>
+        <v>6300</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
@@ -7109,10 +7151,10 @@
       <c r="E133" s="24">
         <v>130</v>
       </c>
-      <c r="F133" s="25">
+      <c r="F133" s="46">
         <v>130</v>
       </c>
-      <c r="G133" s="25">
+      <c r="G133" s="52">
         <v>24</v>
       </c>
       <c r="H133" s="26">
@@ -7121,10 +7163,10 @@
       <c r="I133" s="25">
         <v>94</v>
       </c>
-      <c r="J133" s="25">
+      <c r="J133" s="53">
         <v>154</v>
       </c>
-      <c r="K133" s="25">
+      <c r="K133" s="24">
         <v>24</v>
       </c>
       <c r="L133" s="26">
@@ -7153,10 +7195,10 @@
       <c r="E134" s="24">
         <v>28876</v>
       </c>
-      <c r="F134" s="25">
+      <c r="F134" s="46">
         <v>30864</v>
       </c>
-      <c r="G134" s="25">
+      <c r="G134" s="52">
         <v>978</v>
       </c>
       <c r="H134" s="26">
@@ -7165,10 +7207,10 @@
       <c r="I134" s="25">
         <v>2450</v>
       </c>
-      <c r="J134" s="25">
-        <v>9882</v>
-      </c>
-      <c r="K134" s="25">
+      <c r="J134" s="53">
+        <v>9880</v>
+      </c>
+      <c r="K134" s="24">
         <v>1110</v>
       </c>
       <c r="L134" s="26">
@@ -7178,7 +7220,7 @@
         <v>2660</v>
       </c>
       <c r="N134" s="25">
-        <v>11377</v>
+        <v>11375</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
@@ -7197,10 +7239,10 @@
       <c r="E135" s="24">
         <v>454</v>
       </c>
-      <c r="F135" s="25">
+      <c r="F135" s="46">
         <v>454</v>
       </c>
-      <c r="G135" s="25">
+      <c r="G135" s="52">
         <v>31</v>
       </c>
       <c r="H135" s="26">
@@ -7209,10 +7251,10 @@
       <c r="I135" s="25">
         <v>54</v>
       </c>
-      <c r="J135" s="25">
+      <c r="J135" s="53">
         <v>102</v>
       </c>
-      <c r="K135" s="25">
+      <c r="K135" s="24">
         <v>31</v>
       </c>
       <c r="L135" s="26">
@@ -7241,10 +7283,10 @@
       <c r="E136" s="24">
         <v>1534</v>
       </c>
-      <c r="F136" s="25">
+      <c r="F136" s="46">
         <v>1534</v>
       </c>
-      <c r="G136" s="25">
+      <c r="G136" s="52">
         <v>101</v>
       </c>
       <c r="H136" s="26">
@@ -7253,10 +7295,10 @@
       <c r="I136" s="25">
         <v>562</v>
       </c>
-      <c r="J136" s="25">
+      <c r="J136" s="53">
         <v>1393</v>
       </c>
-      <c r="K136" s="25">
+      <c r="K136" s="24">
         <v>101</v>
       </c>
       <c r="L136" s="26">
@@ -7285,10 +7327,10 @@
       <c r="E137" s="24">
         <v>1063</v>
       </c>
-      <c r="F137" s="25">
+      <c r="F137" s="46">
         <v>1063</v>
       </c>
-      <c r="G137" s="25">
+      <c r="G137" s="52">
         <v>15</v>
       </c>
       <c r="H137" s="26">
@@ -7297,10 +7339,10 @@
       <c r="I137" s="25">
         <v>39</v>
       </c>
-      <c r="J137" s="25">
+      <c r="J137" s="53">
         <v>99</v>
       </c>
-      <c r="K137" s="25">
+      <c r="K137" s="24">
         <v>15</v>
       </c>
       <c r="L137" s="26">
@@ -7329,10 +7371,10 @@
       <c r="E138" s="24">
         <v>0</v>
       </c>
-      <c r="F138" s="25">
+      <c r="F138" s="46">
         <v>0</v>
       </c>
-      <c r="G138" s="25">
+      <c r="G138" s="52">
         <v>685</v>
       </c>
       <c r="H138" s="26">
@@ -7341,10 +7383,10 @@
       <c r="I138" s="25">
         <v>1088</v>
       </c>
-      <c r="J138" s="25">
-        <v>2475</v>
-      </c>
-      <c r="K138" s="25">
+      <c r="J138" s="53">
+        <v>2473</v>
+      </c>
+      <c r="K138" s="24">
         <v>685</v>
       </c>
       <c r="L138" s="26">
@@ -7354,7 +7396,7 @@
         <v>1088</v>
       </c>
       <c r="N138" s="25">
-        <v>2475</v>
+        <v>2473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>